<commit_message>
variabel scope and operators
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -11394,6 +11394,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11420,9 +11423,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -26906,7 +26906,7 @@
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="48"/>
-      <c r="N3" s="343" t="s">
+      <c r="N3" s="344" t="s">
         <v>2991</v>
       </c>
       <c r="O3" s="51"/>
@@ -26935,7 +26935,7 @@
       <c r="K4" s="51"/>
       <c r="L4" s="50"/>
       <c r="M4" s="51"/>
-      <c r="N4" s="344"/>
+      <c r="N4" s="345"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="52"/>
@@ -26961,7 +26961,7 @@
       <c r="M5" s="51" t="s">
         <v>559</v>
       </c>
-      <c r="N5" s="344"/>
+      <c r="N5" s="345"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="52"/>
@@ -26983,7 +26983,7 @@
       <c r="M6" s="54">
         <v>12345</v>
       </c>
-      <c r="N6" s="344"/>
+      <c r="N6" s="345"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="52"/>
@@ -27001,7 +27001,7 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="344"/>
+      <c r="N7" s="345"/>
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="52"/>
@@ -27021,7 +27021,7 @@
       </c>
       <c r="L8" s="47"/>
       <c r="M8" s="48"/>
-      <c r="N8" s="344"/>
+      <c r="N8" s="345"/>
       <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="52"/>
@@ -27039,7 +27039,7 @@
       <c r="K9" s="51"/>
       <c r="L9" s="50"/>
       <c r="M9" s="51"/>
-      <c r="N9" s="344"/>
+      <c r="N9" s="345"/>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="52"/>
@@ -27056,7 +27056,7 @@
       <c r="M10" s="51" t="s">
         <v>524</v>
       </c>
-      <c r="N10" s="344"/>
+      <c r="N10" s="345"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
@@ -27076,7 +27076,7 @@
       <c r="M11" s="54">
         <v>12346</v>
       </c>
-      <c r="N11" s="345"/>
+      <c r="N11" s="346"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="52"/>
@@ -39406,24 +39406,24 @@
     <row r="17" spans="1:14" s="108" customFormat="1"/>
     <row r="22" spans="1:14" ht="15.75" thickBot="1">
       <c r="A22" s="106"/>
-      <c r="B22" s="346" t="s">
+      <c r="B22" s="347" t="s">
         <v>1251</v>
       </c>
-      <c r="C22" s="346"/>
+      <c r="C22" s="347"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106"/>
-      <c r="F22" s="346" t="s">
+      <c r="F22" s="347" t="s">
         <v>1355</v>
       </c>
-      <c r="G22" s="346"/>
-      <c r="H22" s="346"/>
+      <c r="G22" s="347"/>
+      <c r="H22" s="347"/>
       <c r="I22" s="106"/>
       <c r="J22" s="106"/>
-      <c r="K22" s="346" t="s">
+      <c r="K22" s="347" t="s">
         <v>1253</v>
       </c>
-      <c r="L22" s="346"/>
-      <c r="M22" s="346"/>
+      <c r="L22" s="347"/>
+      <c r="M22" s="347"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14">
@@ -41981,35 +41981,35 @@
       </c>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="348" t="s">
+      <c r="B8" s="349" t="s">
         <v>3081</v>
       </c>
-      <c r="C8" s="348"/>
-      <c r="F8" s="348" t="s">
+      <c r="C8" s="349"/>
+      <c r="F8" s="349" t="s">
         <v>3082</v>
       </c>
-      <c r="G8" s="348"/>
-      <c r="I8" s="348" t="s">
+      <c r="G8" s="349"/>
+      <c r="I8" s="349" t="s">
         <v>3082</v>
       </c>
-      <c r="J8" s="348"/>
+      <c r="J8" s="349"/>
       <c r="M8" s="249" t="s">
         <v>3139</v>
       </c>
     </row>
     <row r="9" spans="1:31">
-      <c r="F9" s="348" t="s">
+      <c r="F9" s="349" t="s">
         <v>3083</v>
       </c>
-      <c r="G9" s="348"/>
-      <c r="I9" s="348" t="s">
+      <c r="G9" s="349"/>
+      <c r="I9" s="349" t="s">
         <v>3084</v>
       </c>
-      <c r="J9" s="348"/>
-      <c r="M9" s="349" t="s">
+      <c r="J9" s="349"/>
+      <c r="M9" s="350" t="s">
         <v>3082</v>
       </c>
-      <c r="N9" s="349"/>
+      <c r="N9" s="350"/>
     </row>
     <row r="10" spans="1:31">
       <c r="M10" s="316" t="s">
@@ -42018,19 +42018,19 @@
       <c r="N10" s="316"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="E11" s="347" t="s">
+      <c r="E11" s="348" t="s">
         <v>3086</v>
       </c>
-      <c r="F11" s="347"/>
-      <c r="G11" s="347"/>
-      <c r="H11" s="347"/>
-      <c r="I11" s="347"/>
-      <c r="J11" s="347"/>
-      <c r="K11" s="347"/>
-      <c r="L11" s="347"/>
-      <c r="M11" s="347"/>
-      <c r="N11" s="347"/>
-      <c r="O11" s="347"/>
+      <c r="F11" s="348"/>
+      <c r="G11" s="348"/>
+      <c r="H11" s="348"/>
+      <c r="I11" s="348"/>
+      <c r="J11" s="348"/>
+      <c r="K11" s="348"/>
+      <c r="L11" s="348"/>
+      <c r="M11" s="348"/>
+      <c r="N11" s="348"/>
+      <c r="O11" s="348"/>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" t="s">
@@ -45790,11 +45790,11 @@
       <c r="L6" s="43" t="s">
         <v>1527</v>
       </c>
-      <c r="M6" s="350" t="s">
+      <c r="M6" s="351" t="s">
         <v>1528</v>
       </c>
-      <c r="N6" s="350"/>
-      <c r="O6" s="350"/>
+      <c r="N6" s="351"/>
+      <c r="O6" s="351"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
@@ -51304,8 +51304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51323,23 +51323,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="342" t="s">
+      <c r="A1" s="343" t="s">
         <v>2826</v>
       </c>
-      <c r="B1" s="342"/>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="342"/>
-      <c r="F1" s="342"/>
-      <c r="I1" s="342" t="s">
+      <c r="B1" s="343"/>
+      <c r="C1" s="343"/>
+      <c r="D1" s="343"/>
+      <c r="E1" s="343"/>
+      <c r="F1" s="343"/>
+      <c r="I1" s="343" t="s">
         <v>2838</v>
       </c>
-      <c r="J1" s="342"/>
-      <c r="K1" s="342"/>
-      <c r="L1" s="342"/>
-      <c r="M1" s="342"/>
-      <c r="N1" s="342"/>
-      <c r="O1" s="342"/>
+      <c r="J1" s="343"/>
+      <c r="K1" s="343"/>
+      <c r="L1" s="343"/>
+      <c r="M1" s="343"/>
+      <c r="N1" s="343"/>
+      <c r="O1" s="343"/>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
@@ -51498,24 +51498,24 @@
       <c r="A12" s="335" t="s">
         <v>2840</v>
       </c>
-      <c r="B12" s="341"/>
-      <c r="C12" s="341"/>
-      <c r="D12" s="341"/>
-      <c r="E12" s="341"/>
-      <c r="F12" s="341"/>
-      <c r="G12" s="341"/>
+      <c r="B12" s="342"/>
+      <c r="C12" s="342"/>
+      <c r="D12" s="342"/>
+      <c r="E12" s="342"/>
+      <c r="F12" s="342"/>
+      <c r="G12" s="342"/>
       <c r="H12" s="336"/>
       <c r="I12" s="335" t="s">
         <v>2840</v>
       </c>
-      <c r="J12" s="341"/>
-      <c r="K12" s="341"/>
-      <c r="L12" s="341"/>
-      <c r="M12" s="341"/>
-      <c r="N12" s="341"/>
-      <c r="O12" s="341"/>
-      <c r="P12" s="341"/>
-      <c r="Q12" s="341"/>
+      <c r="J12" s="342"/>
+      <c r="K12" s="342"/>
+      <c r="L12" s="342"/>
+      <c r="M12" s="342"/>
+      <c r="N12" s="342"/>
+      <c r="O12" s="342"/>
+      <c r="P12" s="342"/>
+      <c r="Q12" s="342"/>
       <c r="R12" s="336"/>
     </row>
     <row r="13" spans="1:18">
@@ -51744,14 +51744,14 @@
       <c r="R21" s="37"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="342" t="s">
+      <c r="A24" s="343" t="s">
         <v>2826</v>
       </c>
-      <c r="B24" s="342"/>
-      <c r="C24" s="342"/>
-      <c r="D24" s="342"/>
-      <c r="E24" s="342"/>
-      <c r="F24" s="342"/>
+      <c r="B24" s="343"/>
+      <c r="C24" s="343"/>
+      <c r="D24" s="343"/>
+      <c r="E24" s="343"/>
+      <c r="F24" s="343"/>
       <c r="H24" s="273" t="s">
         <v>2838</v>
       </c>
@@ -51761,11 +51761,11 @@
       <c r="L24" s="273"/>
       <c r="M24" s="273"/>
       <c r="N24" s="273"/>
-      <c r="P24" s="342" t="s">
+      <c r="P24" s="343" t="s">
         <v>2879</v>
       </c>
-      <c r="Q24" s="342"/>
-      <c r="R24" s="342"/>
+      <c r="Q24" s="343"/>
+      <c r="R24" s="343"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="106" t="s">
@@ -52008,24 +52008,24 @@
       <c r="A35" s="335" t="s">
         <v>2880</v>
       </c>
-      <c r="B35" s="341"/>
-      <c r="C35" s="341"/>
-      <c r="D35" s="341"/>
-      <c r="E35" s="341"/>
-      <c r="F35" s="341"/>
-      <c r="G35" s="341"/>
+      <c r="B35" s="342"/>
+      <c r="C35" s="342"/>
+      <c r="D35" s="342"/>
+      <c r="E35" s="342"/>
+      <c r="F35" s="342"/>
+      <c r="G35" s="342"/>
       <c r="H35" s="336"/>
       <c r="I35" s="335" t="s">
         <v>1131</v>
       </c>
-      <c r="J35" s="341"/>
-      <c r="K35" s="341"/>
-      <c r="L35" s="341"/>
-      <c r="M35" s="341"/>
-      <c r="N35" s="341"/>
-      <c r="O35" s="341"/>
-      <c r="P35" s="341"/>
-      <c r="Q35" s="341"/>
+      <c r="J35" s="342"/>
+      <c r="K35" s="342"/>
+      <c r="L35" s="342"/>
+      <c r="M35" s="342"/>
+      <c r="N35" s="342"/>
+      <c r="O35" s="342"/>
+      <c r="P35" s="342"/>
+      <c r="Q35" s="342"/>
       <c r="R35" s="336"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1">
@@ -52906,7 +52906,7 @@
       <c r="A76" t="s">
         <v>144</v>
       </c>
-      <c r="F76" s="351" t="s">
+      <c r="F76" s="341" t="s">
         <v>2110</v>
       </c>
       <c r="G76" s="327"/>

</xml_diff>

<commit_message>
control flow and  constructor
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="references-latest" sheetId="28" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6220" uniqueCount="3263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6253" uniqueCount="3270">
   <si>
     <t>USER</t>
   </si>
@@ -10095,6 +10095,27 @@
   </si>
   <si>
     <t>balance=balance+deposit</t>
+  </si>
+  <si>
+    <t>CLASS IS BLUE-PRINT</t>
+  </si>
+  <si>
+    <t>public Student(String n,int a) {</t>
+  </si>
+  <si>
+    <t>age=a;</t>
+  </si>
+  <si>
+    <t>Student s1=new Student("john",10);</t>
+  </si>
+  <si>
+    <t>// constructor call</t>
+  </si>
+  <si>
+    <t>Student s2=new Student("jane",11);</t>
+  </si>
+  <si>
+    <t>Student s3=new Student("mike",12);</t>
   </si>
 </sst>
 </file>
@@ -19067,7 +19088,7 @@
   <dimension ref="C3:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F67"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19329,8 +19350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20660,10 +20681,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P229"/>
+  <dimension ref="A1:P327"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20672,110 +20693,138 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A1" s="165" t="s">
+        <v>3263</v>
+      </c>
+      <c r="B1" s="165"/>
+      <c r="E1" s="78" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>1432</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>549</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>413</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="J2" s="47"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>1781</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="27" t="s">
-        <v>2944</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>1432</v>
-      </c>
+      <c r="B3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>550</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>2629</v>
+      </c>
+      <c r="G3" s="27"/>
       <c r="H3" s="27"/>
-      <c r="I3" s="27" t="s">
-        <v>413</v>
-      </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>412</v>
+      </c>
+      <c r="L3" s="27"/>
       <c r="M3" s="34"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="E4" s="33"/>
-      <c r="F4" s="27" t="s">
-        <v>1804</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>413</v>
-      </c>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B4" t="s">
+        <v>707</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>709</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>2631</v>
+      </c>
+      <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>524</v>
-      </c>
+      <c r="J4" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="55">
+        <v>10</v>
+      </c>
+      <c r="L4" s="27"/>
       <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="B5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E5" s="33"/>
-      <c r="F5" s="27" t="s">
-        <v>1790</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>1951</v>
-      </c>
+        <v>3264</v>
+      </c>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="37"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B6" t="s">
-        <v>2939</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="38" t="s">
-        <v>2363</v>
-      </c>
-      <c r="G6" s="38" t="s">
+    <row r="6" spans="1:13">
+      <c r="C6" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27" t="s">
         <v>2629</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="27"/>
       <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13">
       <c r="C7" t="s">
-        <v>2940</v>
+        <v>3265</v>
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="27"/>
-      <c r="I7" s="27" t="s">
-        <v>1951</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="32"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="52" t="s">
+        <v>524</v>
+      </c>
+      <c r="L7" s="27"/>
       <c r="M7" s="34"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1">
       <c r="B8" t="s">
         <v>144</v>
       </c>
@@ -20784,37 +20833,39 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="L8" s="34" t="s">
-        <v>559</v>
-      </c>
+      <c r="J8" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="K8" s="55">
+        <v>11</v>
+      </c>
+      <c r="L8" s="27"/>
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A9" t="s">
-        <v>144</v>
-      </c>
       <c r="E9" s="33"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="37"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="34"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1">
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
       <c r="E10" s="33"/>
       <c r="F10" s="27"/>
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="27" t="s">
+        <v>2631</v>
+      </c>
+      <c r="J10" s="47"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="27"/>
       <c r="M10" s="34"/>
     </row>
@@ -20823,49 +20874,51 @@
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
-      <c r="I11" s="27" t="s">
-        <v>2629</v>
-      </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="52" t="s">
+        <v>559</v>
+      </c>
+      <c r="L11" s="27"/>
       <c r="M11" s="34"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="A12" t="s">
-        <v>2941</v>
+        <v>3266</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="34" t="s">
-        <v>1025</v>
-      </c>
+      <c r="J12" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="K12" s="55">
+        <v>12</v>
+      </c>
+      <c r="L12" s="27"/>
       <c r="M12" s="34"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>2942</v>
+        <v>3267</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="37"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>2943</v>
+        <v>3268</v>
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="27"/>
@@ -20878,6 +20931,9 @@
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>3269</v>
+      </c>
       <c r="E15" s="33"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
@@ -20888,1332 +20944,1633 @@
       <c r="L15" s="27"/>
       <c r="M15" s="34"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1">
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="37"/>
-    </row>
-    <row r="19" spans="16:16" ht="15.75" thickBot="1"/>
-    <row r="20" spans="16:16">
+    <row r="16" spans="1:13">
+      <c r="E16" s="33"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="34"/>
+    </row>
+    <row r="17" spans="5:16">
+      <c r="E17" s="33"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="34"/>
+    </row>
+    <row r="18" spans="5:16" ht="15.75" thickBot="1">
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="37"/>
+    </row>
+    <row r="19" spans="5:16" ht="15.75" thickBot="1"/>
+    <row r="20" spans="5:16">
       <c r="P20" s="32"/>
     </row>
-    <row r="21" spans="16:16">
+    <row r="21" spans="5:16">
       <c r="P21" s="34"/>
     </row>
-    <row r="22" spans="16:16">
+    <row r="22" spans="5:16">
       <c r="P22" s="34"/>
     </row>
-    <row r="23" spans="16:16">
+    <row r="23" spans="5:16">
       <c r="P23" s="34"/>
     </row>
-    <row r="24" spans="16:16">
+    <row r="24" spans="5:16">
       <c r="P24" s="34"/>
     </row>
-    <row r="25" spans="16:16">
+    <row r="25" spans="5:16">
       <c r="P25" s="34"/>
     </row>
-    <row r="26" spans="16:16">
+    <row r="26" spans="5:16">
       <c r="P26" s="34"/>
     </row>
-    <row r="27" spans="16:16">
+    <row r="27" spans="5:16">
       <c r="P27" s="34"/>
     </row>
-    <row r="28" spans="16:16" ht="15.75" thickBot="1">
+    <row r="28" spans="5:16" ht="15.75" thickBot="1">
       <c r="P28" s="37"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A118" t="s">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" ht="15.75" thickBot="1">
-      <c r="B119" t="s">
-        <v>1689</v>
-      </c>
-      <c r="F119" s="47" t="s">
-        <v>1939</v>
-      </c>
-      <c r="G119" s="48" t="s">
+    <row r="99" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="100" spans="1:13" ht="15.75" thickBot="1">
+      <c r="E100" s="30"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="31"/>
+      <c r="K100" s="31"/>
+      <c r="L100" s="31"/>
+      <c r="M100" s="32"/>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E101" s="33"/>
+      <c r="F101" s="27" t="s">
+        <v>2944</v>
+      </c>
+      <c r="G101" s="27" t="s">
+        <v>1432</v>
+      </c>
+      <c r="H101" s="27"/>
+      <c r="I101" s="27" t="s">
         <v>413</v>
       </c>
-      <c r="H119" s="48"/>
-      <c r="I119" s="48"/>
-      <c r="J119" s="48"/>
-      <c r="K119" s="48"/>
-      <c r="L119" s="49"/>
-    </row>
-    <row r="120" spans="1:12">
-      <c r="B120" t="s">
-        <v>2046</v>
-      </c>
-      <c r="F120" s="50" t="s">
-        <v>1940</v>
-      </c>
-      <c r="G120" s="51" t="s">
-        <v>517</v>
-      </c>
-      <c r="H120" s="51"/>
-      <c r="I120" s="51" t="s">
+      <c r="J101" s="30"/>
+      <c r="K101" s="31"/>
+      <c r="L101" s="32"/>
+      <c r="M101" s="34"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="E102" s="33"/>
+      <c r="F102" s="27" t="s">
+        <v>1804</v>
+      </c>
+      <c r="G102" s="27" t="s">
         <v>413</v>
       </c>
-      <c r="J120" s="47" t="s">
-        <v>1694</v>
-      </c>
-      <c r="K120" s="49" t="s">
-        <v>1848</v>
-      </c>
-      <c r="L120" s="52"/>
-    </row>
-    <row r="121" spans="1:12">
-      <c r="B121" t="s">
-        <v>2047</v>
-      </c>
-      <c r="F121" s="50" t="s">
-        <v>1943</v>
-      </c>
-      <c r="G121" s="51" t="s">
-        <v>2051</v>
-      </c>
-      <c r="H121" s="51"/>
-      <c r="I121" s="51"/>
-      <c r="J121" s="50" t="s">
-        <v>1698</v>
-      </c>
-      <c r="K121" s="52" t="s">
-        <v>2050</v>
-      </c>
-      <c r="L121" s="52"/>
-    </row>
-    <row r="122" spans="1:12">
-      <c r="B122" t="s">
-        <v>2048</v>
-      </c>
-      <c r="F122" s="50" t="s">
-        <v>1944</v>
-      </c>
-      <c r="G122" s="51" t="s">
-        <v>519</v>
-      </c>
-      <c r="H122" s="51"/>
-      <c r="I122" s="51"/>
-      <c r="J122" s="50" t="s">
-        <v>2049</v>
-      </c>
-      <c r="K122" s="52">
-        <v>4</v>
-      </c>
-      <c r="L122" s="52"/>
-    </row>
-    <row r="123" spans="1:12" ht="15.75" thickBot="1">
-      <c r="F123" s="50"/>
-      <c r="G123" s="51"/>
-      <c r="H123" s="51"/>
-      <c r="I123" s="51"/>
-      <c r="J123" s="53" t="s">
-        <v>1697</v>
-      </c>
-      <c r="K123" s="55">
-        <v>1234</v>
-      </c>
-      <c r="L123" s="52"/>
-    </row>
-    <row r="124" spans="1:12" ht="15.75" thickBot="1">
-      <c r="B124" t="s">
-        <v>2052</v>
-      </c>
-      <c r="F124" s="50"/>
-      <c r="G124" s="51"/>
-      <c r="H124" s="51"/>
-      <c r="I124" s="51"/>
-      <c r="J124" s="51"/>
-      <c r="K124" s="51"/>
-      <c r="L124" s="52"/>
-    </row>
-    <row r="125" spans="1:12">
-      <c r="C125" t="s">
-        <v>2053</v>
-      </c>
-      <c r="F125" s="50"/>
-      <c r="G125" s="51"/>
-      <c r="H125" s="51"/>
-      <c r="I125" s="51" t="s">
-        <v>517</v>
-      </c>
-      <c r="J125" s="47" t="s">
-        <v>1694</v>
-      </c>
-      <c r="K125" s="49" t="s">
-        <v>2057</v>
-      </c>
-      <c r="L125" s="52"/>
-    </row>
-    <row r="126" spans="1:12">
-      <c r="B126" t="s">
+      <c r="H102" s="27"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="33"/>
+      <c r="K102" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L102" s="34" t="s">
+        <v>524</v>
+      </c>
+      <c r="M102" s="34"/>
+    </row>
+    <row r="103" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B103" t="s">
+        <v>356</v>
+      </c>
+      <c r="E103" s="33"/>
+      <c r="F103" s="27" t="s">
+        <v>1790</v>
+      </c>
+      <c r="G103" s="27" t="s">
+        <v>1951</v>
+      </c>
+      <c r="H103" s="27"/>
+      <c r="I103" s="27"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="36"/>
+      <c r="L103" s="37"/>
+      <c r="M103" s="34"/>
+    </row>
+    <row r="104" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B104" t="s">
+        <v>2939</v>
+      </c>
+      <c r="E104" s="33"/>
+      <c r="F104" s="38" t="s">
+        <v>2363</v>
+      </c>
+      <c r="G104" s="38" t="s">
+        <v>2629</v>
+      </c>
+      <c r="H104" s="27"/>
+      <c r="I104" s="27"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="27"/>
+      <c r="M104" s="34"/>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="C105" t="s">
+        <v>2940</v>
+      </c>
+      <c r="E105" s="33"/>
+      <c r="F105" s="27"/>
+      <c r="G105" s="27"/>
+      <c r="H105" s="27"/>
+      <c r="I105" s="27" t="s">
+        <v>1951</v>
+      </c>
+      <c r="J105" s="30"/>
+      <c r="K105" s="31"/>
+      <c r="L105" s="32"/>
+      <c r="M105" s="34"/>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="B106" t="s">
         <v>144</v>
       </c>
-      <c r="F126" s="50"/>
-      <c r="G126" s="51"/>
-      <c r="H126" s="51"/>
-      <c r="I126" s="51"/>
-      <c r="J126" s="50" t="s">
-        <v>1698</v>
-      </c>
-      <c r="K126" s="52" t="s">
-        <v>2050</v>
-      </c>
-      <c r="L126" s="52"/>
-    </row>
-    <row r="127" spans="1:12">
-      <c r="B127" t="s">
-        <v>2060</v>
-      </c>
-      <c r="F127" s="50"/>
-      <c r="G127" s="51"/>
-      <c r="H127" s="51"/>
-      <c r="I127" s="51"/>
-      <c r="J127" s="50" t="s">
-        <v>2049</v>
-      </c>
-      <c r="K127" s="52">
-        <v>2</v>
-      </c>
-      <c r="L127" s="52"/>
-    </row>
-    <row r="128" spans="1:12" ht="15.75" thickBot="1">
-      <c r="C128" t="s">
-        <v>2053</v>
-      </c>
-      <c r="F128" s="50"/>
-      <c r="G128" s="51"/>
-      <c r="H128" s="51"/>
-      <c r="I128" s="51"/>
-      <c r="J128" s="53" t="s">
-        <v>1697</v>
-      </c>
-      <c r="K128" s="55">
-        <v>1234</v>
-      </c>
-      <c r="L128" s="52"/>
-    </row>
-    <row r="129" spans="1:15" ht="15.75" thickBot="1">
-      <c r="C129" t="s">
-        <v>2061</v>
-      </c>
-      <c r="F129" s="50"/>
-      <c r="G129" s="51"/>
-      <c r="H129" s="51"/>
-      <c r="I129" s="51"/>
-      <c r="J129" s="51"/>
-      <c r="K129" s="51"/>
-      <c r="L129" s="52"/>
-    </row>
-    <row r="130" spans="1:15">
-      <c r="B130" t="s">
+      <c r="E106" s="33"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
+      <c r="H106" s="27"/>
+      <c r="I106" s="27"/>
+      <c r="J106" s="33"/>
+      <c r="K106" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L106" s="34" t="s">
+        <v>559</v>
+      </c>
+      <c r="M106" s="34"/>
+    </row>
+    <row r="107" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A107" t="s">
         <v>144</v>
       </c>
-      <c r="F130" s="191" t="s">
-        <v>519</v>
-      </c>
-      <c r="G130" s="47" t="s">
-        <v>1694</v>
-      </c>
-      <c r="H130" s="49" t="s">
-        <v>2059</v>
-      </c>
-      <c r="I130" s="51" t="s">
-        <v>2051</v>
-      </c>
-      <c r="J130" s="47" t="s">
-        <v>1694</v>
-      </c>
-      <c r="K130" s="49" t="s">
-        <v>2058</v>
-      </c>
-      <c r="L130" s="52"/>
-    </row>
-    <row r="131" spans="1:15">
-      <c r="A131" t="s">
-        <v>144</v>
-      </c>
-      <c r="F131" s="191"/>
-      <c r="G131" s="50" t="s">
-        <v>1698</v>
-      </c>
-      <c r="H131" s="52" t="s">
-        <v>2050</v>
-      </c>
-      <c r="I131" s="51"/>
-      <c r="J131" s="50" t="s">
-        <v>1698</v>
-      </c>
-      <c r="K131" s="52" t="s">
-        <v>2050</v>
-      </c>
-      <c r="L131" s="52"/>
-    </row>
-    <row r="132" spans="1:15">
-      <c r="A132" t="s">
-        <v>2054</v>
-      </c>
-      <c r="F132" s="191"/>
-      <c r="G132" s="50" t="s">
-        <v>2049</v>
-      </c>
-      <c r="H132" s="52">
-        <v>4</v>
-      </c>
-      <c r="I132" s="51"/>
-      <c r="J132" s="50" t="s">
-        <v>2049</v>
-      </c>
-      <c r="K132" s="52">
-        <v>4</v>
-      </c>
-      <c r="L132" s="52"/>
-    </row>
-    <row r="133" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A133" t="s">
-        <v>2062</v>
-      </c>
-      <c r="F133" s="191"/>
-      <c r="G133" s="53" t="s">
-        <v>1697</v>
-      </c>
-      <c r="H133" s="55">
-        <v>1234</v>
-      </c>
-      <c r="I133" s="51"/>
-      <c r="J133" s="53" t="s">
-        <v>1697</v>
-      </c>
-      <c r="K133" s="55">
-        <v>1234</v>
-      </c>
-      <c r="L133" s="52"/>
-    </row>
-    <row r="134" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A134" t="s">
-        <v>2055</v>
-      </c>
-      <c r="F134" s="53"/>
-      <c r="G134" s="54"/>
-      <c r="H134" s="54"/>
-      <c r="I134" s="54"/>
-      <c r="J134" s="54"/>
-      <c r="K134" s="54"/>
-      <c r="L134" s="55"/>
-    </row>
-    <row r="135" spans="1:15">
-      <c r="A135" t="s">
-        <v>2056</v>
-      </c>
-    </row>
-    <row r="136" spans="1:15" ht="15.75" thickBot="1"/>
-    <row r="137" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A137" s="30"/>
-      <c r="B137" s="31"/>
-      <c r="C137" s="31"/>
-      <c r="D137" s="31"/>
-      <c r="E137" s="31"/>
-      <c r="F137" s="31"/>
-      <c r="G137" s="31"/>
-      <c r="H137" s="31"/>
-      <c r="I137" s="31"/>
-      <c r="J137" s="31"/>
-      <c r="K137" s="31"/>
-      <c r="L137" s="31"/>
-      <c r="M137" s="31"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="27"/>
+      <c r="I107" s="27"/>
+      <c r="J107" s="35"/>
+      <c r="K107" s="36"/>
+      <c r="L107" s="37"/>
+      <c r="M107" s="34"/>
+    </row>
+    <row r="108" spans="1:13" ht="15.75" thickBot="1">
+      <c r="E108" s="33"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
+      <c r="H108" s="27"/>
+      <c r="I108" s="27"/>
+      <c r="J108" s="27"/>
+      <c r="K108" s="27"/>
+      <c r="L108" s="27"/>
+      <c r="M108" s="34"/>
+    </row>
+    <row r="109" spans="1:13">
+      <c r="E109" s="33"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27" t="s">
+        <v>2629</v>
+      </c>
+      <c r="J109" s="30"/>
+      <c r="K109" s="31"/>
+      <c r="L109" s="32"/>
+      <c r="M109" s="34"/>
+    </row>
+    <row r="110" spans="1:13">
+      <c r="A110" t="s">
+        <v>2941</v>
+      </c>
+      <c r="E110" s="33"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
+      <c r="H110" s="27"/>
+      <c r="I110" s="27"/>
+      <c r="J110" s="33"/>
+      <c r="K110" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L110" s="34" t="s">
+        <v>1025</v>
+      </c>
+      <c r="M110" s="34"/>
+    </row>
+    <row r="111" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A111" t="s">
+        <v>2942</v>
+      </c>
+      <c r="E111" s="33"/>
+      <c r="F111" s="27"/>
+      <c r="G111" s="27"/>
+      <c r="H111" s="27"/>
+      <c r="I111" s="27"/>
+      <c r="J111" s="35"/>
+      <c r="K111" s="36"/>
+      <c r="L111" s="37"/>
+      <c r="M111" s="34"/>
+    </row>
+    <row r="112" spans="1:13">
+      <c r="A112" t="s">
+        <v>2943</v>
+      </c>
+      <c r="E112" s="33"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="27"/>
+      <c r="I112" s="27"/>
+      <c r="J112" s="27"/>
+      <c r="K112" s="27"/>
+      <c r="L112" s="27"/>
+      <c r="M112" s="34"/>
+    </row>
+    <row r="113" spans="5:13">
+      <c r="E113" s="33"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
+      <c r="J113" s="27"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="27"/>
+      <c r="M113" s="34"/>
+    </row>
+    <row r="114" spans="5:13" ht="15.75" thickBot="1">
+      <c r="E114" s="35"/>
+      <c r="F114" s="36"/>
+      <c r="G114" s="36"/>
+      <c r="H114" s="36"/>
+      <c r="I114" s="36"/>
+      <c r="J114" s="36"/>
+      <c r="K114" s="36"/>
+      <c r="L114" s="36"/>
+      <c r="M114" s="37"/>
+    </row>
+    <row r="136" spans="14:15" ht="15.75" thickBot="1"/>
+    <row r="137" spans="14:15">
       <c r="N137" s="31"/>
       <c r="O137" s="31"/>
     </row>
-    <row r="138" spans="1:15">
-      <c r="A138" s="33"/>
-      <c r="B138" s="27"/>
-      <c r="C138" s="27"/>
-      <c r="D138" s="27"/>
-      <c r="E138" s="27"/>
-      <c r="F138" s="27" t="s">
-        <v>517</v>
-      </c>
-      <c r="G138" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="H138" s="49" t="s">
-        <v>559</v>
-      </c>
-      <c r="I138" s="27"/>
-      <c r="J138" s="27"/>
-      <c r="K138" s="27"/>
-      <c r="L138" s="27"/>
-      <c r="M138" s="27"/>
+    <row r="138" spans="14:15">
       <c r="N138" s="27"/>
       <c r="O138" s="27"/>
     </row>
-    <row r="139" spans="1:15">
-      <c r="A139" s="33"/>
-      <c r="B139" s="27" t="s">
-        <v>549</v>
-      </c>
-      <c r="C139" s="27" t="s">
-        <v>517</v>
-      </c>
-      <c r="D139" s="27"/>
-      <c r="E139" s="27"/>
-      <c r="F139" s="27"/>
-      <c r="G139" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="H139" s="52">
-        <v>10</v>
-      </c>
-      <c r="I139" s="27"/>
-      <c r="J139" s="27"/>
-      <c r="K139" s="27"/>
-      <c r="L139" s="27"/>
-      <c r="M139" s="27"/>
+    <row r="139" spans="14:15">
       <c r="N139" s="27"/>
       <c r="O139" s="27"/>
     </row>
-    <row r="140" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A140" s="33"/>
-      <c r="B140" s="27"/>
-      <c r="C140" s="27"/>
-      <c r="D140" s="27"/>
-      <c r="E140" s="27"/>
-      <c r="F140" s="27"/>
-      <c r="G140" s="53" t="s">
-        <v>190</v>
-      </c>
-      <c r="H140" s="55">
-        <v>3</v>
-      </c>
-      <c r="I140" s="27"/>
-      <c r="J140" s="27"/>
-      <c r="K140" s="27"/>
-      <c r="L140" s="27"/>
-      <c r="M140" s="27"/>
+    <row r="140" spans="14:15">
       <c r="N140" s="27"/>
       <c r="O140" s="27"/>
     </row>
-    <row r="141" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A141" s="33"/>
-      <c r="B141" s="27" t="s">
-        <v>550</v>
-      </c>
-      <c r="C141" s="27" t="s">
-        <v>519</v>
-      </c>
-      <c r="D141" s="27"/>
-      <c r="E141" s="51"/>
-      <c r="F141" s="51"/>
-      <c r="G141" s="51"/>
-      <c r="H141" s="27"/>
-      <c r="I141" s="27"/>
-      <c r="J141" s="51"/>
-      <c r="K141" s="51"/>
-      <c r="L141" s="27"/>
-      <c r="M141" s="27"/>
+    <row r="141" spans="14:15">
       <c r="N141" s="27"/>
       <c r="O141" s="27"/>
     </row>
-    <row r="142" spans="1:15">
-      <c r="A142" s="33"/>
-      <c r="B142" s="27"/>
-      <c r="C142" s="27"/>
-      <c r="D142" s="27"/>
-      <c r="E142" s="51"/>
-      <c r="F142" s="27"/>
-      <c r="G142" s="47"/>
-      <c r="H142" s="49"/>
-      <c r="I142" s="27"/>
-      <c r="J142" s="74"/>
-      <c r="K142" s="47"/>
-      <c r="L142" s="49"/>
-      <c r="M142" s="38"/>
+    <row r="142" spans="14:15">
       <c r="N142" s="27"/>
       <c r="O142" s="27"/>
     </row>
-    <row r="143" spans="1:15">
-      <c r="A143" s="33"/>
-      <c r="B143" s="27" t="s">
-        <v>709</v>
-      </c>
-      <c r="C143" s="27" t="s">
-        <v>551</v>
-      </c>
-      <c r="D143" s="27"/>
-      <c r="E143" s="51"/>
-      <c r="F143" s="27"/>
-      <c r="G143" s="50"/>
-      <c r="H143" s="52"/>
-      <c r="I143" s="27"/>
-      <c r="J143" s="27"/>
-      <c r="K143" s="50"/>
-      <c r="L143" s="52"/>
-      <c r="M143" s="27"/>
+    <row r="143" spans="14:15">
       <c r="N143" s="27"/>
       <c r="O143" s="27"/>
     </row>
-    <row r="144" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A144" s="33"/>
-      <c r="B144" s="27"/>
-      <c r="C144" s="27"/>
-      <c r="D144" s="27"/>
-      <c r="E144" s="27"/>
-      <c r="F144" s="27"/>
-      <c r="G144" s="53"/>
-      <c r="H144" s="55"/>
-      <c r="I144" s="27"/>
-      <c r="J144" s="27"/>
-      <c r="K144" s="53"/>
-      <c r="L144" s="55"/>
-      <c r="M144" s="27"/>
+    <row r="144" spans="14:15">
       <c r="N144" s="27"/>
       <c r="O144" s="27"/>
     </row>
-    <row r="145" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A145" s="35"/>
-      <c r="B145" s="36"/>
-      <c r="C145" s="36"/>
-      <c r="D145" s="36"/>
-      <c r="E145" s="36"/>
-      <c r="F145" s="36"/>
-      <c r="G145" s="36"/>
-      <c r="H145" s="36"/>
-      <c r="I145" s="36"/>
-      <c r="J145" s="36"/>
-      <c r="K145" s="36"/>
-      <c r="L145" s="36"/>
-      <c r="M145" s="36"/>
+    <row r="145" spans="14:15" ht="15.75" thickBot="1">
       <c r="N145" s="36"/>
       <c r="O145" s="36"/>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="14:15">
       <c r="O147" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
-      <c r="A148" t="s">
-        <v>703</v>
-      </c>
+    <row r="148" spans="14:15">
       <c r="O148" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
-      <c r="B149" t="s">
-        <v>704</v>
-      </c>
-      <c r="G149" t="s">
-        <v>706</v>
-      </c>
+    <row r="149" spans="14:15">
       <c r="O149" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
-      <c r="C150" t="s">
-        <v>710</v>
-      </c>
-      <c r="H150" t="s">
-        <v>356</v>
-      </c>
+    <row r="150" spans="14:15">
       <c r="O150" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
-      <c r="C151" t="s">
+    <row r="170" spans="14:14" ht="15.75" thickBot="1"/>
+    <row r="171" spans="14:14">
+      <c r="N171" s="32"/>
+    </row>
+    <row r="172" spans="14:14">
+      <c r="N172" s="34"/>
+    </row>
+    <row r="173" spans="14:14">
+      <c r="N173" s="34"/>
+    </row>
+    <row r="174" spans="14:14">
+      <c r="N174" s="34"/>
+    </row>
+    <row r="175" spans="14:14">
+      <c r="N175" s="34"/>
+    </row>
+    <row r="176" spans="14:14">
+      <c r="N176" s="34"/>
+    </row>
+    <row r="177" spans="14:14">
+      <c r="N177" s="34"/>
+    </row>
+    <row r="178" spans="14:14">
+      <c r="N178" s="34"/>
+    </row>
+    <row r="179" spans="14:14">
+      <c r="N179" s="34"/>
+    </row>
+    <row r="180" spans="14:14">
+      <c r="N180" s="34"/>
+    </row>
+    <row r="181" spans="14:14">
+      <c r="N181" s="34"/>
+    </row>
+    <row r="182" spans="14:14">
+      <c r="N182" s="34"/>
+    </row>
+    <row r="183" spans="14:14" ht="15.75" thickBot="1">
+      <c r="N183" s="37"/>
+    </row>
+    <row r="216" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A216" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B217" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F217" s="47" t="s">
+        <v>1939</v>
+      </c>
+      <c r="G217" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="H217" s="48"/>
+      <c r="I217" s="48"/>
+      <c r="J217" s="48"/>
+      <c r="K217" s="48"/>
+      <c r="L217" s="49"/>
+    </row>
+    <row r="218" spans="1:12">
+      <c r="B218" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F218" s="50" t="s">
+        <v>1940</v>
+      </c>
+      <c r="G218" s="51" t="s">
+        <v>517</v>
+      </c>
+      <c r="H218" s="51"/>
+      <c r="I218" s="51" t="s">
+        <v>413</v>
+      </c>
+      <c r="J218" s="47" t="s">
+        <v>1694</v>
+      </c>
+      <c r="K218" s="49" t="s">
+        <v>1848</v>
+      </c>
+      <c r="L218" s="52"/>
+    </row>
+    <row r="219" spans="1:12">
+      <c r="B219" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F219" s="50" t="s">
+        <v>1943</v>
+      </c>
+      <c r="G219" s="51" t="s">
+        <v>2051</v>
+      </c>
+      <c r="H219" s="51"/>
+      <c r="I219" s="51"/>
+      <c r="J219" s="50" t="s">
+        <v>1698</v>
+      </c>
+      <c r="K219" s="52" t="s">
+        <v>2050</v>
+      </c>
+      <c r="L219" s="52"/>
+    </row>
+    <row r="220" spans="1:12">
+      <c r="B220" t="s">
+        <v>2048</v>
+      </c>
+      <c r="F220" s="50" t="s">
+        <v>1944</v>
+      </c>
+      <c r="G220" s="51" t="s">
+        <v>519</v>
+      </c>
+      <c r="H220" s="51"/>
+      <c r="I220" s="51"/>
+      <c r="J220" s="50" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K220" s="52">
+        <v>4</v>
+      </c>
+      <c r="L220" s="52"/>
+    </row>
+    <row r="221" spans="1:12" ht="15.75" thickBot="1">
+      <c r="F221" s="50"/>
+      <c r="G221" s="51"/>
+      <c r="H221" s="51"/>
+      <c r="I221" s="51"/>
+      <c r="J221" s="53" t="s">
+        <v>1697</v>
+      </c>
+      <c r="K221" s="55">
+        <v>1234</v>
+      </c>
+      <c r="L221" s="52"/>
+    </row>
+    <row r="222" spans="1:12" ht="15.75" thickBot="1">
+      <c r="B222" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F222" s="50"/>
+      <c r="G222" s="51"/>
+      <c r="H222" s="51"/>
+      <c r="I222" s="51"/>
+      <c r="J222" s="51"/>
+      <c r="K222" s="51"/>
+      <c r="L222" s="52"/>
+    </row>
+    <row r="223" spans="1:12">
+      <c r="C223" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F223" s="50"/>
+      <c r="G223" s="51"/>
+      <c r="H223" s="51"/>
+      <c r="I223" s="51" t="s">
+        <v>517</v>
+      </c>
+      <c r="J223" s="47" t="s">
+        <v>1694</v>
+      </c>
+      <c r="K223" s="49" t="s">
+        <v>2057</v>
+      </c>
+      <c r="L223" s="52"/>
+    </row>
+    <row r="224" spans="1:12">
+      <c r="B224" t="s">
+        <v>144</v>
+      </c>
+      <c r="F224" s="50"/>
+      <c r="G224" s="51"/>
+      <c r="H224" s="51"/>
+      <c r="I224" s="51"/>
+      <c r="J224" s="50" t="s">
+        <v>1698</v>
+      </c>
+      <c r="K224" s="52" t="s">
+        <v>2050</v>
+      </c>
+      <c r="L224" s="52"/>
+    </row>
+    <row r="225" spans="1:13">
+      <c r="B225" t="s">
+        <v>2060</v>
+      </c>
+      <c r="F225" s="50"/>
+      <c r="G225" s="51"/>
+      <c r="H225" s="51"/>
+      <c r="I225" s="51"/>
+      <c r="J225" s="50" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K225" s="52">
+        <v>2</v>
+      </c>
+      <c r="L225" s="52"/>
+    </row>
+    <row r="226" spans="1:13" ht="15.75" thickBot="1">
+      <c r="C226" t="s">
+        <v>2053</v>
+      </c>
+      <c r="F226" s="50"/>
+      <c r="G226" s="51"/>
+      <c r="H226" s="51"/>
+      <c r="I226" s="51"/>
+      <c r="J226" s="53" t="s">
+        <v>1697</v>
+      </c>
+      <c r="K226" s="55">
+        <v>1234</v>
+      </c>
+      <c r="L226" s="52"/>
+    </row>
+    <row r="227" spans="1:13" ht="15.75" thickBot="1">
+      <c r="C227" t="s">
+        <v>2061</v>
+      </c>
+      <c r="F227" s="50"/>
+      <c r="G227" s="51"/>
+      <c r="H227" s="51"/>
+      <c r="I227" s="51"/>
+      <c r="J227" s="51"/>
+      <c r="K227" s="51"/>
+      <c r="L227" s="52"/>
+    </row>
+    <row r="228" spans="1:13">
+      <c r="B228" t="s">
+        <v>144</v>
+      </c>
+      <c r="F228" s="191" t="s">
+        <v>519</v>
+      </c>
+      <c r="G228" s="47" t="s">
+        <v>1694</v>
+      </c>
+      <c r="H228" s="49" t="s">
+        <v>2059</v>
+      </c>
+      <c r="I228" s="51" t="s">
+        <v>2051</v>
+      </c>
+      <c r="J228" s="47" t="s">
+        <v>1694</v>
+      </c>
+      <c r="K228" s="49" t="s">
+        <v>2058</v>
+      </c>
+      <c r="L228" s="52"/>
+    </row>
+    <row r="229" spans="1:13">
+      <c r="A229" t="s">
+        <v>144</v>
+      </c>
+      <c r="F229" s="191"/>
+      <c r="G229" s="50" t="s">
+        <v>1698</v>
+      </c>
+      <c r="H229" s="52" t="s">
+        <v>2050</v>
+      </c>
+      <c r="I229" s="51"/>
+      <c r="J229" s="50" t="s">
+        <v>1698</v>
+      </c>
+      <c r="K229" s="52" t="s">
+        <v>2050</v>
+      </c>
+      <c r="L229" s="52"/>
+    </row>
+    <row r="230" spans="1:13">
+      <c r="A230" t="s">
+        <v>2054</v>
+      </c>
+      <c r="F230" s="191"/>
+      <c r="G230" s="50" t="s">
+        <v>2049</v>
+      </c>
+      <c r="H230" s="52">
+        <v>4</v>
+      </c>
+      <c r="I230" s="51"/>
+      <c r="J230" s="50" t="s">
+        <v>2049</v>
+      </c>
+      <c r="K230" s="52">
+        <v>4</v>
+      </c>
+      <c r="L230" s="52"/>
+    </row>
+    <row r="231" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A231" t="s">
+        <v>2062</v>
+      </c>
+      <c r="F231" s="191"/>
+      <c r="G231" s="53" t="s">
+        <v>1697</v>
+      </c>
+      <c r="H231" s="55">
+        <v>1234</v>
+      </c>
+      <c r="I231" s="51"/>
+      <c r="J231" s="53" t="s">
+        <v>1697</v>
+      </c>
+      <c r="K231" s="55">
+        <v>1234</v>
+      </c>
+      <c r="L231" s="52"/>
+    </row>
+    <row r="232" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A232" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F232" s="53"/>
+      <c r="G232" s="54"/>
+      <c r="H232" s="54"/>
+      <c r="I232" s="54"/>
+      <c r="J232" s="54"/>
+      <c r="K232" s="54"/>
+      <c r="L232" s="55"/>
+    </row>
+    <row r="233" spans="1:13">
+      <c r="A233" t="s">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="235" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A235" s="30"/>
+      <c r="B235" s="31"/>
+      <c r="C235" s="31"/>
+      <c r="D235" s="31"/>
+      <c r="E235" s="31"/>
+      <c r="F235" s="31"/>
+      <c r="G235" s="31"/>
+      <c r="H235" s="31"/>
+      <c r="I235" s="31"/>
+      <c r="J235" s="31"/>
+      <c r="K235" s="31"/>
+      <c r="L235" s="31"/>
+      <c r="M235" s="31"/>
+    </row>
+    <row r="236" spans="1:13">
+      <c r="A236" s="33"/>
+      <c r="B236" s="27"/>
+      <c r="C236" s="27"/>
+      <c r="D236" s="27"/>
+      <c r="E236" s="27"/>
+      <c r="F236" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="G236" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="H236" s="49" t="s">
+        <v>559</v>
+      </c>
+      <c r="I236" s="27"/>
+      <c r="J236" s="27"/>
+      <c r="K236" s="27"/>
+      <c r="L236" s="27"/>
+      <c r="M236" s="27"/>
+    </row>
+    <row r="237" spans="1:13">
+      <c r="A237" s="33"/>
+      <c r="B237" s="27" t="s">
+        <v>549</v>
+      </c>
+      <c r="C237" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="D237" s="27"/>
+      <c r="E237" s="27"/>
+      <c r="F237" s="27"/>
+      <c r="G237" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="H237" s="52">
+        <v>10</v>
+      </c>
+      <c r="I237" s="27"/>
+      <c r="J237" s="27"/>
+      <c r="K237" s="27"/>
+      <c r="L237" s="27"/>
+      <c r="M237" s="27"/>
+    </row>
+    <row r="238" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A238" s="33"/>
+      <c r="B238" s="27"/>
+      <c r="C238" s="27"/>
+      <c r="D238" s="27"/>
+      <c r="E238" s="27"/>
+      <c r="F238" s="27"/>
+      <c r="G238" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="H238" s="55">
+        <v>3</v>
+      </c>
+      <c r="I238" s="27"/>
+      <c r="J238" s="27"/>
+      <c r="K238" s="27"/>
+      <c r="L238" s="27"/>
+      <c r="M238" s="27"/>
+    </row>
+    <row r="239" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A239" s="33"/>
+      <c r="B239" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="C239" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="D239" s="27"/>
+      <c r="E239" s="51"/>
+      <c r="F239" s="51"/>
+      <c r="G239" s="51"/>
+      <c r="H239" s="27"/>
+      <c r="I239" s="27"/>
+      <c r="J239" s="51"/>
+      <c r="K239" s="51"/>
+      <c r="L239" s="27"/>
+      <c r="M239" s="27"/>
+    </row>
+    <row r="240" spans="1:13">
+      <c r="A240" s="33"/>
+      <c r="B240" s="27"/>
+      <c r="C240" s="27"/>
+      <c r="D240" s="27"/>
+      <c r="E240" s="51"/>
+      <c r="F240" s="27"/>
+      <c r="G240" s="47"/>
+      <c r="H240" s="49"/>
+      <c r="I240" s="27"/>
+      <c r="J240" s="74"/>
+      <c r="K240" s="47"/>
+      <c r="L240" s="49"/>
+      <c r="M240" s="38"/>
+    </row>
+    <row r="241" spans="1:13">
+      <c r="A241" s="33"/>
+      <c r="B241" s="27" t="s">
+        <v>709</v>
+      </c>
+      <c r="C241" s="27" t="s">
+        <v>551</v>
+      </c>
+      <c r="D241" s="27"/>
+      <c r="E241" s="51"/>
+      <c r="F241" s="27"/>
+      <c r="G241" s="50"/>
+      <c r="H241" s="52"/>
+      <c r="I241" s="27"/>
+      <c r="J241" s="27"/>
+      <c r="K241" s="50"/>
+      <c r="L241" s="52"/>
+      <c r="M241" s="27"/>
+    </row>
+    <row r="242" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A242" s="33"/>
+      <c r="B242" s="27"/>
+      <c r="C242" s="27"/>
+      <c r="D242" s="27"/>
+      <c r="E242" s="27"/>
+      <c r="F242" s="27"/>
+      <c r="G242" s="53"/>
+      <c r="H242" s="55"/>
+      <c r="I242" s="27"/>
+      <c r="J242" s="27"/>
+      <c r="K242" s="53"/>
+      <c r="L242" s="55"/>
+      <c r="M242" s="27"/>
+    </row>
+    <row r="243" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A243" s="35"/>
+      <c r="B243" s="36"/>
+      <c r="C243" s="36"/>
+      <c r="D243" s="36"/>
+      <c r="E243" s="36"/>
+      <c r="F243" s="36"/>
+      <c r="G243" s="36"/>
+      <c r="H243" s="36"/>
+      <c r="I243" s="36"/>
+      <c r="J243" s="36"/>
+      <c r="K243" s="36"/>
+      <c r="L243" s="36"/>
+      <c r="M243" s="36"/>
+    </row>
+    <row r="246" spans="1:13">
+      <c r="A246" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13">
+      <c r="B247" t="s">
+        <v>704</v>
+      </c>
+      <c r="G247" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13">
+      <c r="C248" t="s">
+        <v>710</v>
+      </c>
+      <c r="H248" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13">
+      <c r="C249" t="s">
         <v>711</v>
       </c>
-      <c r="H151" t="s">
+      <c r="H249" t="s">
         <v>707</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
-      <c r="C152" t="s">
+    <row r="250" spans="1:13">
+      <c r="C250" t="s">
         <v>712</v>
       </c>
-      <c r="H152" t="s">
+      <c r="H250" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
-      <c r="C153" t="s">
+    <row r="251" spans="1:13">
+      <c r="C251" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="154" spans="1:15">
-      <c r="C154" t="s">
+    <row r="252" spans="1:13">
+      <c r="C252" t="s">
         <v>568</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H252" t="s">
         <v>714</v>
       </c>
-      <c r="J154" t="s">
+      <c r="J252" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
-      <c r="C155" t="s">
+    <row r="253" spans="1:13">
+      <c r="C253" t="s">
         <v>705</v>
       </c>
-      <c r="I155" t="s">
+      <c r="I253" t="s">
         <v>716</v>
       </c>
-      <c r="J155" t="s">
+      <c r="J253" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="156" spans="1:15">
-      <c r="B156" t="s">
+    <row r="254" spans="1:13">
+      <c r="B254" t="s">
         <v>144</v>
       </c>
-      <c r="H156" t="s">
+      <c r="H254" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
-      <c r="A157" t="s">
+    <row r="255" spans="1:13">
+      <c r="A255" t="s">
         <v>144</v>
       </c>
-      <c r="G157" t="s">
+      <c r="G255" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="160" spans="1:15">
-      <c r="A160" t="s">
+    <row r="258" spans="1:13">
+      <c r="A258" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="161" spans="1:14">
-      <c r="A161" t="s">
+    <row r="259" spans="1:13">
+      <c r="A259" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="162" spans="1:14">
-      <c r="A162" t="s">
+    <row r="260" spans="1:13">
+      <c r="A260" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="163" spans="1:14">
-      <c r="G163" t="s">
+    <row r="261" spans="1:13">
+      <c r="G261" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="164" spans="1:14">
-      <c r="H164" t="s">
+    <row r="262" spans="1:13">
+      <c r="H262" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="165" spans="1:14">
-      <c r="G165" t="s">
+    <row r="263" spans="1:13">
+      <c r="G263" t="s">
         <v>718</v>
       </c>
-      <c r="J165" t="s">
+      <c r="J263" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="166" spans="1:14">
-      <c r="J166" t="s">
+    <row r="264" spans="1:13">
+      <c r="J264" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="167" spans="1:14">
-      <c r="I167" t="s">
+    <row r="265" spans="1:13">
+      <c r="I265" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="168" spans="1:14">
-      <c r="I168" t="s">
+    <row r="266" spans="1:13">
+      <c r="I266" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15.75" thickBot="1"/>
-    <row r="171" spans="1:14">
-      <c r="A171" t="s">
+    <row r="268" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="269" spans="1:13">
+      <c r="A269" t="s">
         <v>1845</v>
       </c>
-      <c r="G171" s="47"/>
-      <c r="H171" s="48"/>
-      <c r="I171" s="48"/>
-      <c r="J171" s="48"/>
-      <c r="K171" s="48"/>
-      <c r="L171" s="48"/>
-      <c r="M171" s="48"/>
-      <c r="N171" s="32"/>
-    </row>
-    <row r="172" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A172" t="s">
+      <c r="G269" s="47"/>
+      <c r="H269" s="48"/>
+      <c r="I269" s="48"/>
+      <c r="J269" s="48"/>
+      <c r="K269" s="48"/>
+      <c r="L269" s="48"/>
+      <c r="M269" s="48"/>
+    </row>
+    <row r="270" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A270" t="s">
         <v>1846</v>
       </c>
-      <c r="G172" s="50" t="s">
+      <c r="G270" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="H172" s="51" t="s">
+      <c r="H270" s="51" t="s">
         <v>1432</v>
       </c>
-      <c r="I172" s="51"/>
-      <c r="J172" s="51"/>
-      <c r="K172" s="51"/>
-      <c r="L172" s="51"/>
-      <c r="M172" s="51"/>
-      <c r="N172" s="34"/>
-    </row>
-    <row r="173" spans="1:14">
-      <c r="G173" s="50" t="s">
+      <c r="I270" s="51"/>
+      <c r="J270" s="51"/>
+      <c r="K270" s="51"/>
+      <c r="L270" s="51"/>
+      <c r="M270" s="51"/>
+    </row>
+    <row r="271" spans="1:13">
+      <c r="G271" s="50" t="s">
         <v>412</v>
       </c>
-      <c r="H173" s="51" t="s">
+      <c r="H271" s="51" t="s">
         <v>429</v>
       </c>
-      <c r="I173" s="51"/>
-      <c r="J173" s="51" t="s">
+      <c r="I271" s="51"/>
+      <c r="J271" s="51" t="s">
         <v>429</v>
       </c>
-      <c r="K173" s="47" t="s">
+      <c r="K271" s="47" t="s">
         <v>1694</v>
       </c>
-      <c r="L173" s="49" t="s">
+      <c r="L271" s="49" t="s">
         <v>1695</v>
       </c>
-      <c r="M173" s="51"/>
-      <c r="N173" s="34"/>
-    </row>
-    <row r="174" spans="1:14">
-      <c r="A174" t="s">
+      <c r="M271" s="51"/>
+    </row>
+    <row r="272" spans="1:13">
+      <c r="A272" t="s">
         <v>1692</v>
       </c>
-      <c r="G174" s="50"/>
-      <c r="H174" s="51"/>
-      <c r="I174" s="51"/>
-      <c r="J174" s="51" t="s">
+      <c r="G272" s="50"/>
+      <c r="H272" s="51"/>
+      <c r="I272" s="51"/>
+      <c r="J272" s="51" t="s">
         <v>1851</v>
       </c>
-      <c r="K174" s="50" t="s">
+      <c r="K272" s="50" t="s">
         <v>1697</v>
       </c>
-      <c r="L174" s="52">
+      <c r="L272" s="52">
         <v>123</v>
       </c>
-      <c r="M174" s="51"/>
-      <c r="N174" s="34"/>
-    </row>
-    <row r="175" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A175" t="s">
+      <c r="M272" s="51"/>
+    </row>
+    <row r="273" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A273" t="s">
         <v>1693</v>
       </c>
-      <c r="G175" s="50"/>
-      <c r="H175" s="51"/>
-      <c r="I175" s="51"/>
-      <c r="J175" s="51"/>
-      <c r="K175" s="53" t="s">
+      <c r="G273" s="50"/>
+      <c r="H273" s="51"/>
+      <c r="I273" s="51"/>
+      <c r="J273" s="51"/>
+      <c r="K273" s="53" t="s">
         <v>1698</v>
       </c>
-      <c r="L175" s="55" t="s">
+      <c r="L273" s="55" t="s">
         <v>1696</v>
       </c>
-      <c r="M175" s="51"/>
-      <c r="N175" s="34"/>
-    </row>
-    <row r="176" spans="1:14">
-      <c r="G176" s="50"/>
-      <c r="H176" s="51"/>
-      <c r="I176" s="51"/>
-      <c r="J176" s="51"/>
-      <c r="K176" s="51"/>
-      <c r="L176" s="51"/>
-      <c r="M176" s="51"/>
-      <c r="N176" s="34"/>
-    </row>
-    <row r="177" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A177" t="s">
+      <c r="M273" s="51"/>
+    </row>
+    <row r="274" spans="1:13">
+      <c r="G274" s="50"/>
+      <c r="H274" s="51"/>
+      <c r="I274" s="51"/>
+      <c r="J274" s="51"/>
+      <c r="K274" s="51"/>
+      <c r="L274" s="51"/>
+      <c r="M274" s="51"/>
+    </row>
+    <row r="275" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A275" t="s">
         <v>1688</v>
       </c>
-      <c r="G177" s="50"/>
-      <c r="H177" s="51"/>
-      <c r="I177" s="51"/>
-      <c r="J177" s="51"/>
-      <c r="K177" s="51"/>
-      <c r="L177" s="51"/>
-      <c r="M177" s="51"/>
-      <c r="N177" s="34"/>
-    </row>
-    <row r="178" spans="1:14">
-      <c r="B178" t="s">
+      <c r="G275" s="50"/>
+      <c r="H275" s="51"/>
+      <c r="I275" s="51"/>
+      <c r="J275" s="51"/>
+      <c r="K275" s="51"/>
+      <c r="L275" s="51"/>
+      <c r="M275" s="51"/>
+    </row>
+    <row r="276" spans="1:13">
+      <c r="B276" t="s">
         <v>1689</v>
       </c>
-      <c r="G178" s="50"/>
-      <c r="H178" s="51"/>
-      <c r="I178" s="51"/>
-      <c r="J178" s="51" t="s">
+      <c r="G276" s="50"/>
+      <c r="H276" s="51"/>
+      <c r="I276" s="51"/>
+      <c r="J276" s="51" t="s">
         <v>1844</v>
       </c>
-      <c r="K178" s="47" t="s">
+      <c r="K276" s="47" t="s">
         <v>1694</v>
       </c>
-      <c r="L178" s="49" t="s">
+      <c r="L276" s="49" t="s">
         <v>1848</v>
       </c>
-      <c r="M178" s="51"/>
-      <c r="N178" s="34"/>
-    </row>
-    <row r="179" spans="1:14">
-      <c r="B179" t="s">
+      <c r="M276" s="51"/>
+    </row>
+    <row r="277" spans="1:13">
+      <c r="B277" t="s">
         <v>1690</v>
       </c>
-      <c r="G179" s="50"/>
-      <c r="H179" s="51"/>
-      <c r="I179" s="51"/>
-      <c r="J179" s="51"/>
-      <c r="K179" s="50" t="s">
+      <c r="G277" s="50"/>
+      <c r="H277" s="51"/>
+      <c r="I277" s="51"/>
+      <c r="J277" s="51"/>
+      <c r="K277" s="50" t="s">
         <v>1697</v>
       </c>
-      <c r="L179" s="52">
+      <c r="L277" s="52">
         <v>223</v>
       </c>
-      <c r="M179" s="51"/>
-      <c r="N179" s="34"/>
-    </row>
-    <row r="180" spans="1:14" ht="15.75" thickBot="1">
-      <c r="B180" t="s">
+      <c r="M277" s="51"/>
+    </row>
+    <row r="278" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B278" t="s">
         <v>1691</v>
       </c>
-      <c r="G180" s="50"/>
-      <c r="H180" s="51"/>
-      <c r="I180" s="51"/>
-      <c r="J180" s="51"/>
-      <c r="K180" s="53" t="s">
+      <c r="G278" s="50"/>
+      <c r="H278" s="51"/>
+      <c r="I278" s="51"/>
+      <c r="J278" s="51"/>
+      <c r="K278" s="53" t="s">
         <v>1698</v>
       </c>
-      <c r="L180" s="55" t="s">
+      <c r="L278" s="55" t="s">
         <v>1696</v>
       </c>
-      <c r="M180" s="51"/>
-      <c r="N180" s="34"/>
-    </row>
-    <row r="181" spans="1:14">
-      <c r="G181" s="50"/>
-      <c r="H181" s="51"/>
-      <c r="I181" s="51"/>
-      <c r="J181" s="51"/>
-      <c r="K181" s="51"/>
-      <c r="L181" s="51"/>
-      <c r="M181" s="51"/>
-      <c r="N181" s="34"/>
-    </row>
-    <row r="182" spans="1:14">
-      <c r="B182" t="s">
+      <c r="M278" s="51"/>
+    </row>
+    <row r="279" spans="1:13">
+      <c r="G279" s="50"/>
+      <c r="H279" s="51"/>
+      <c r="I279" s="51"/>
+      <c r="J279" s="51"/>
+      <c r="K279" s="51"/>
+      <c r="L279" s="51"/>
+      <c r="M279" s="51"/>
+    </row>
+    <row r="280" spans="1:13">
+      <c r="B280" t="s">
         <v>1849</v>
       </c>
-      <c r="G182" s="33"/>
-      <c r="H182" s="27"/>
-      <c r="I182" s="27"/>
-      <c r="J182" s="27"/>
-      <c r="K182" s="27"/>
-      <c r="L182" s="27"/>
-      <c r="M182" s="27"/>
-      <c r="N182" s="34"/>
-    </row>
-    <row r="183" spans="1:14" ht="15.75" thickBot="1">
-      <c r="C183" t="s">
+      <c r="G280" s="33"/>
+      <c r="H280" s="27"/>
+      <c r="I280" s="27"/>
+      <c r="J280" s="27"/>
+      <c r="K280" s="27"/>
+      <c r="L280" s="27"/>
+      <c r="M280" s="27"/>
+    </row>
+    <row r="281" spans="1:13" ht="15.75" thickBot="1">
+      <c r="C281" t="s">
         <v>1850</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D281" t="s">
         <v>1852</v>
       </c>
-      <c r="G183" s="35"/>
-      <c r="H183" s="36"/>
-      <c r="I183" s="36"/>
-      <c r="J183" s="36"/>
-      <c r="K183" s="36"/>
-      <c r="L183" s="36"/>
-      <c r="M183" s="36"/>
-      <c r="N183" s="37"/>
-    </row>
-    <row r="184" spans="1:14">
-      <c r="C184" t="s">
+      <c r="G281" s="35"/>
+      <c r="H281" s="36"/>
+      <c r="I281" s="36"/>
+      <c r="J281" s="36"/>
+      <c r="K281" s="36"/>
+      <c r="L281" s="36"/>
+      <c r="M281" s="36"/>
+    </row>
+    <row r="282" spans="1:13">
+      <c r="C282" t="s">
         <v>1847</v>
       </c>
     </row>
-    <row r="185" spans="1:14">
-      <c r="B185" t="s">
+    <row r="283" spans="1:13">
+      <c r="B283" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="187" spans="1:14">
-      <c r="A187" t="s">
+    <row r="285" spans="1:13">
+      <c r="A285" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="188" spans="1:14">
-      <c r="F188" s="29" t="s">
+    <row r="286" spans="1:13">
+      <c r="F286" s="29" t="s">
         <v>1853</v>
       </c>
-      <c r="G188" s="29"/>
-      <c r="H188" s="29" t="s">
+      <c r="G286" s="29"/>
+      <c r="H286" s="29" t="s">
         <v>1854</v>
       </c>
     </row>
-    <row r="189" spans="1:14">
-      <c r="G189" s="29" t="s">
+    <row r="287" spans="1:13">
+      <c r="G287" s="29" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="15.75" thickBot="1"/>
-    <row r="191" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A191" t="s">
+    <row r="288" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="289" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A289" t="s">
         <v>1856</v>
       </c>
-      <c r="G191" s="30" t="s">
+      <c r="G289" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="H191" s="31" t="s">
+      <c r="H289" s="31" t="s">
         <v>1432</v>
       </c>
-      <c r="I191" s="31"/>
-      <c r="J191" s="31"/>
-      <c r="K191" s="31"/>
-      <c r="L191" s="31"/>
-      <c r="M191" s="32"/>
-    </row>
-    <row r="192" spans="1:14">
-      <c r="B192" t="s">
+      <c r="I289" s="31"/>
+      <c r="J289" s="31"/>
+      <c r="K289" s="31"/>
+      <c r="L289" s="31"/>
+      <c r="M289" s="32"/>
+    </row>
+    <row r="290" spans="1:13">
+      <c r="B290" t="s">
         <v>1857</v>
       </c>
-      <c r="G192" s="33" t="s">
+      <c r="G290" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="H192" s="27"/>
-      <c r="I192" s="27"/>
-      <c r="J192" s="27" t="s">
+      <c r="H290" s="27"/>
+      <c r="I290" s="27"/>
+      <c r="J290" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="K192" s="30" t="s">
+      <c r="K290" s="30" t="s">
         <v>1862</v>
       </c>
-      <c r="L192" s="32">
+      <c r="L290" s="32">
         <v>150</v>
       </c>
-      <c r="M192" s="34"/>
-    </row>
-    <row r="193" spans="1:13">
-      <c r="G193" s="33"/>
-      <c r="H193" s="27"/>
-      <c r="I193" s="27"/>
-      <c r="J193" s="27"/>
-      <c r="K193" s="33"/>
-      <c r="L193" s="34"/>
-      <c r="M193" s="34"/>
-    </row>
-    <row r="194" spans="1:13">
-      <c r="B194" t="s">
+      <c r="M290" s="34"/>
+    </row>
+    <row r="291" spans="1:13">
+      <c r="G291" s="33"/>
+      <c r="H291" s="27"/>
+      <c r="I291" s="27"/>
+      <c r="J291" s="27"/>
+      <c r="K291" s="33"/>
+      <c r="L291" s="34"/>
+      <c r="M291" s="34"/>
+    </row>
+    <row r="292" spans="1:13">
+      <c r="B292" t="s">
         <v>1860</v>
       </c>
-      <c r="G194" s="33"/>
-      <c r="H194" s="27"/>
-      <c r="I194" s="27"/>
-      <c r="J194" s="27"/>
-      <c r="K194" s="33"/>
-      <c r="L194" s="34"/>
-      <c r="M194" s="34"/>
-    </row>
-    <row r="195" spans="1:13">
-      <c r="C195" t="s">
+      <c r="G292" s="33"/>
+      <c r="H292" s="27"/>
+      <c r="I292" s="27"/>
+      <c r="J292" s="27"/>
+      <c r="K292" s="33"/>
+      <c r="L292" s="34"/>
+      <c r="M292" s="34"/>
+    </row>
+    <row r="293" spans="1:13">
+      <c r="C293" t="s">
         <v>1861</v>
       </c>
-      <c r="G195" s="33"/>
-      <c r="H195" s="27"/>
-      <c r="I195" s="27"/>
-      <c r="J195" s="27"/>
-      <c r="K195" s="33"/>
-      <c r="L195" s="34"/>
-      <c r="M195" s="34"/>
-    </row>
-    <row r="196" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B196" t="s">
+      <c r="G293" s="33"/>
+      <c r="H293" s="27"/>
+      <c r="I293" s="27"/>
+      <c r="J293" s="27"/>
+      <c r="K293" s="33"/>
+      <c r="L293" s="34"/>
+      <c r="M293" s="34"/>
+    </row>
+    <row r="294" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B294" t="s">
         <v>144</v>
       </c>
-      <c r="G196" s="33"/>
-      <c r="H196" s="27"/>
-      <c r="I196" s="27"/>
-      <c r="J196" s="27"/>
-      <c r="K196" s="35"/>
-      <c r="L196" s="37"/>
-      <c r="M196" s="34"/>
-    </row>
-    <row r="197" spans="1:13">
-      <c r="A197" t="s">
+      <c r="G294" s="33"/>
+      <c r="H294" s="27"/>
+      <c r="I294" s="27"/>
+      <c r="J294" s="27"/>
+      <c r="K294" s="35"/>
+      <c r="L294" s="37"/>
+      <c r="M294" s="34"/>
+    </row>
+    <row r="295" spans="1:13">
+      <c r="A295" t="s">
         <v>144</v>
       </c>
-      <c r="G197" s="33"/>
-      <c r="H197" s="27"/>
-      <c r="I197" s="27"/>
-      <c r="J197" s="27"/>
-      <c r="K197" s="27"/>
-      <c r="L197" s="27"/>
-      <c r="M197" s="34"/>
-    </row>
-    <row r="198" spans="1:13">
-      <c r="G198" s="33"/>
-      <c r="H198" s="27"/>
-      <c r="I198" s="27"/>
-      <c r="J198" s="27"/>
-      <c r="K198" s="27"/>
-      <c r="L198" s="27"/>
-      <c r="M198" s="34"/>
-    </row>
-    <row r="199" spans="1:13">
-      <c r="A199" t="s">
+      <c r="G295" s="33"/>
+      <c r="H295" s="27"/>
+      <c r="I295" s="27"/>
+      <c r="J295" s="27"/>
+      <c r="K295" s="27"/>
+      <c r="L295" s="27"/>
+      <c r="M295" s="34"/>
+    </row>
+    <row r="296" spans="1:13">
+      <c r="G296" s="33"/>
+      <c r="H296" s="27"/>
+      <c r="I296" s="27"/>
+      <c r="J296" s="27"/>
+      <c r="K296" s="27"/>
+      <c r="L296" s="27"/>
+      <c r="M296" s="34"/>
+    </row>
+    <row r="297" spans="1:13">
+      <c r="A297" t="s">
         <v>1855</v>
       </c>
-      <c r="G199" s="33"/>
-      <c r="H199" s="27"/>
-      <c r="I199" s="27"/>
-      <c r="J199" s="27"/>
-      <c r="K199" s="27"/>
-      <c r="L199" s="27"/>
-      <c r="M199" s="34"/>
-    </row>
-    <row r="200" spans="1:13">
-      <c r="B200" t="s">
+      <c r="G297" s="33"/>
+      <c r="H297" s="27"/>
+      <c r="I297" s="27"/>
+      <c r="J297" s="27"/>
+      <c r="K297" s="27"/>
+      <c r="L297" s="27"/>
+      <c r="M297" s="34"/>
+    </row>
+    <row r="298" spans="1:13">
+      <c r="B298" t="s">
         <v>356</v>
       </c>
-      <c r="G200" s="33"/>
-      <c r="H200" s="27"/>
-      <c r="I200" s="27"/>
-      <c r="J200" s="27"/>
-      <c r="K200" s="27"/>
-      <c r="L200" s="27"/>
-      <c r="M200" s="34"/>
-    </row>
-    <row r="201" spans="1:13">
-      <c r="B201" t="s">
+      <c r="G298" s="33"/>
+      <c r="H298" s="27"/>
+      <c r="I298" s="27"/>
+      <c r="J298" s="27"/>
+      <c r="K298" s="27"/>
+      <c r="L298" s="27"/>
+      <c r="M298" s="34"/>
+    </row>
+    <row r="299" spans="1:13">
+      <c r="B299" t="s">
         <v>1858</v>
       </c>
-      <c r="G201" s="33"/>
-      <c r="H201" s="27"/>
-      <c r="I201" s="27"/>
-      <c r="J201" s="27"/>
-      <c r="K201" s="27"/>
-      <c r="L201" s="27"/>
-      <c r="M201" s="34"/>
-    </row>
-    <row r="202" spans="1:13">
-      <c r="C202" t="s">
+      <c r="G299" s="33"/>
+      <c r="H299" s="27"/>
+      <c r="I299" s="27"/>
+      <c r="J299" s="27"/>
+      <c r="K299" s="27"/>
+      <c r="L299" s="27"/>
+      <c r="M299" s="34"/>
+    </row>
+    <row r="300" spans="1:13">
+      <c r="C300" t="s">
         <v>1859</v>
       </c>
-      <c r="G202" s="33"/>
-      <c r="H202" s="27"/>
-      <c r="I202" s="27"/>
-      <c r="J202" s="27"/>
-      <c r="K202" s="27"/>
-      <c r="L202" s="27"/>
-      <c r="M202" s="34"/>
-    </row>
-    <row r="203" spans="1:13">
-      <c r="B203" t="s">
+      <c r="G300" s="33"/>
+      <c r="H300" s="27"/>
+      <c r="I300" s="27"/>
+      <c r="J300" s="27"/>
+      <c r="K300" s="27"/>
+      <c r="L300" s="27"/>
+      <c r="M300" s="34"/>
+    </row>
+    <row r="301" spans="1:13">
+      <c r="B301" t="s">
         <v>144</v>
       </c>
-      <c r="G203" s="33"/>
-      <c r="H203" s="27" t="s">
+      <c r="G301" s="33"/>
+      <c r="H301" s="27" t="s">
         <v>1853</v>
       </c>
-      <c r="I203" s="27" t="s">
+      <c r="I301" s="27" t="s">
         <v>1863</v>
       </c>
-      <c r="J203" s="27"/>
-      <c r="K203" s="27"/>
-      <c r="L203" s="27"/>
-      <c r="M203" s="34"/>
-    </row>
-    <row r="204" spans="1:13">
-      <c r="A204" t="s">
+      <c r="J301" s="27"/>
+      <c r="K301" s="27"/>
+      <c r="L301" s="27"/>
+      <c r="M301" s="34"/>
+    </row>
+    <row r="302" spans="1:13">
+      <c r="A302" t="s">
         <v>144</v>
       </c>
-      <c r="G204" s="33"/>
-      <c r="H204" s="27" t="s">
+      <c r="G302" s="33"/>
+      <c r="H302" s="27" t="s">
         <v>1853</v>
       </c>
-      <c r="I204" s="27" t="s">
+      <c r="I302" s="27" t="s">
         <v>1864</v>
       </c>
-      <c r="J204" s="27"/>
-      <c r="K204" s="27"/>
-      <c r="L204" s="27"/>
-      <c r="M204" s="34"/>
-    </row>
-    <row r="205" spans="1:13">
-      <c r="G205" s="33"/>
-      <c r="H205" s="27"/>
-      <c r="I205" s="27"/>
-      <c r="J205" s="27"/>
-      <c r="K205" s="27"/>
-      <c r="L205" s="27"/>
-      <c r="M205" s="34"/>
-    </row>
-    <row r="206" spans="1:13">
-      <c r="A206" t="s">
+      <c r="J302" s="27"/>
+      <c r="K302" s="27"/>
+      <c r="L302" s="27"/>
+      <c r="M302" s="34"/>
+    </row>
+    <row r="303" spans="1:13">
+      <c r="G303" s="33"/>
+      <c r="H303" s="27"/>
+      <c r="I303" s="27"/>
+      <c r="J303" s="27"/>
+      <c r="K303" s="27"/>
+      <c r="L303" s="27"/>
+      <c r="M303" s="34"/>
+    </row>
+    <row r="304" spans="1:13">
+      <c r="A304" t="s">
         <v>729</v>
       </c>
-      <c r="G206" s="33"/>
-      <c r="H206" s="27" t="s">
+      <c r="G304" s="33"/>
+      <c r="H304" s="27" t="s">
         <v>728</v>
       </c>
-      <c r="I206" s="27" t="s">
+      <c r="I304" s="27" t="s">
         <v>1863</v>
       </c>
-      <c r="J206" s="27"/>
-      <c r="K206" s="27"/>
-      <c r="L206" s="27"/>
-      <c r="M206" s="34"/>
-    </row>
-    <row r="207" spans="1:13" ht="15.75" thickBot="1">
-      <c r="G207" s="35"/>
-      <c r="H207" s="36" t="s">
+      <c r="J304" s="27"/>
+      <c r="K304" s="27"/>
+      <c r="L304" s="27"/>
+      <c r="M304" s="34"/>
+    </row>
+    <row r="305" spans="1:13" ht="15.75" thickBot="1">
+      <c r="G305" s="35"/>
+      <c r="H305" s="36" t="s">
         <v>728</v>
       </c>
-      <c r="I207" s="27" t="s">
+      <c r="I305" s="27" t="s">
         <v>1864</v>
       </c>
-      <c r="J207" s="36"/>
-      <c r="K207" s="36"/>
-      <c r="L207" s="36"/>
-      <c r="M207" s="37"/>
-    </row>
-    <row r="209" spans="1:13">
-      <c r="A209" t="s">
+      <c r="J305" s="36"/>
+      <c r="K305" s="36"/>
+      <c r="L305" s="36"/>
+      <c r="M305" s="37"/>
+    </row>
+    <row r="307" spans="1:13">
+      <c r="A307" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="212" spans="1:13">
-      <c r="A212" t="s">
+    <row r="309" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="310" spans="1:13">
+      <c r="A310" t="s">
         <v>1865</v>
       </c>
-      <c r="G212" s="30"/>
-      <c r="H212" s="31"/>
-      <c r="I212" s="31"/>
-      <c r="J212" s="31"/>
-      <c r="K212" s="31"/>
-      <c r="L212" s="31"/>
-      <c r="M212" s="32"/>
-    </row>
-    <row r="213" spans="1:13" ht="15.75" thickBot="1">
-      <c r="B213" t="s">
+      <c r="G310" s="30"/>
+      <c r="H310" s="31"/>
+      <c r="I310" s="31"/>
+      <c r="J310" s="31"/>
+      <c r="K310" s="31"/>
+      <c r="L310" s="31"/>
+      <c r="M310" s="32"/>
+    </row>
+    <row r="311" spans="1:13" ht="15.75" thickBot="1">
+      <c r="B311" t="s">
         <v>1866</v>
       </c>
-      <c r="G213" s="33"/>
-      <c r="H213" s="38" t="s">
+      <c r="G311" s="33"/>
+      <c r="H311" s="38" t="s">
         <v>760</v>
       </c>
-      <c r="I213" s="39"/>
-      <c r="J213" s="39"/>
-      <c r="K213" s="39"/>
-      <c r="L213" s="39"/>
-      <c r="M213" s="34"/>
-    </row>
-    <row r="214" spans="1:13">
-      <c r="B214" t="s">
+      <c r="I311" s="39"/>
+      <c r="J311" s="39"/>
+      <c r="K311" s="39"/>
+      <c r="L311" s="39"/>
+      <c r="M311" s="34"/>
+    </row>
+    <row r="312" spans="1:13">
+      <c r="B312" t="s">
         <v>1867</v>
       </c>
-      <c r="G214" s="33"/>
-      <c r="H214" s="38"/>
-      <c r="I214" s="30" t="s">
+      <c r="G312" s="33"/>
+      <c r="H312" s="38"/>
+      <c r="I312" s="30" t="s">
         <v>1880</v>
       </c>
-      <c r="J214" s="31"/>
-      <c r="K214" s="32"/>
-      <c r="L214" s="39"/>
-      <c r="M214" s="34"/>
-    </row>
-    <row r="215" spans="1:13">
-      <c r="C215" t="s">
+      <c r="J312" s="31"/>
+      <c r="K312" s="32"/>
+      <c r="L312" s="39"/>
+      <c r="M312" s="34"/>
+    </row>
+    <row r="313" spans="1:13">
+      <c r="C313" t="s">
         <v>1868</v>
       </c>
-      <c r="G215" s="33"/>
-      <c r="H215" s="131"/>
-      <c r="I215" s="166" t="s">
+      <c r="G313" s="33"/>
+      <c r="H313" s="131"/>
+      <c r="I313" s="166" t="s">
         <v>21</v>
       </c>
-      <c r="J215" s="27"/>
-      <c r="K215" s="34"/>
-      <c r="L215" s="39"/>
-      <c r="M215" s="34"/>
-    </row>
-    <row r="216" spans="1:13">
-      <c r="B216" t="s">
+      <c r="J313" s="27"/>
+      <c r="K313" s="34"/>
+      <c r="L313" s="39"/>
+      <c r="M313" s="34"/>
+    </row>
+    <row r="314" spans="1:13">
+      <c r="B314" t="s">
         <v>144</v>
       </c>
-      <c r="G216" s="33"/>
-      <c r="H216" s="131"/>
-      <c r="I216" s="43" t="s">
+      <c r="G314" s="33"/>
+      <c r="H314" s="131"/>
+      <c r="I314" s="43" t="s">
         <v>1876</v>
       </c>
-      <c r="J216" s="27"/>
-      <c r="K216" s="34"/>
-      <c r="L216" s="39"/>
-      <c r="M216" s="34"/>
-    </row>
-    <row r="217" spans="1:13">
-      <c r="B217" t="s">
+      <c r="J314" s="27"/>
+      <c r="K314" s="34"/>
+      <c r="L314" s="39"/>
+      <c r="M314" s="34"/>
+    </row>
+    <row r="315" spans="1:13">
+      <c r="B315" t="s">
         <v>1869</v>
       </c>
-      <c r="G217" s="33"/>
-      <c r="H217" s="38"/>
-      <c r="I217" s="33"/>
-      <c r="J217" s="27"/>
-      <c r="K217" s="34"/>
-      <c r="L217" s="39"/>
-      <c r="M217" s="34"/>
-    </row>
-    <row r="218" spans="1:13">
-      <c r="C218" t="s">
+      <c r="G315" s="33"/>
+      <c r="H315" s="38"/>
+      <c r="I315" s="33"/>
+      <c r="J315" s="27"/>
+      <c r="K315" s="34"/>
+      <c r="L315" s="39"/>
+      <c r="M315" s="34"/>
+    </row>
+    <row r="316" spans="1:13">
+      <c r="C316" t="s">
         <v>1870</v>
       </c>
-      <c r="G218" s="33"/>
-      <c r="H218" s="131"/>
-      <c r="I218" s="166" t="s">
+      <c r="G316" s="33"/>
+      <c r="H316" s="131"/>
+      <c r="I316" s="166" t="s">
         <v>1877</v>
       </c>
-      <c r="J218" s="27"/>
-      <c r="K218" s="34"/>
-      <c r="L218" s="39"/>
-      <c r="M218" s="34"/>
-    </row>
-    <row r="219" spans="1:13">
-      <c r="B219" t="s">
+      <c r="J316" s="27"/>
+      <c r="K316" s="34"/>
+      <c r="L316" s="39"/>
+      <c r="M316" s="34"/>
+    </row>
+    <row r="317" spans="1:13">
+      <c r="B317" t="s">
         <v>144</v>
       </c>
-      <c r="G219" s="33"/>
-      <c r="H219" s="131"/>
-      <c r="I219" s="166" t="s">
+      <c r="G317" s="33"/>
+      <c r="H317" s="131"/>
+      <c r="I317" s="166" t="s">
         <v>1879</v>
       </c>
-      <c r="J219" s="27"/>
-      <c r="K219" s="34"/>
-      <c r="L219" s="39"/>
-      <c r="M219" s="34"/>
-    </row>
-    <row r="220" spans="1:13">
-      <c r="A220" t="s">
+      <c r="J317" s="27"/>
+      <c r="K317" s="34"/>
+      <c r="L317" s="39"/>
+      <c r="M317" s="34"/>
+    </row>
+    <row r="318" spans="1:13">
+      <c r="A318" t="s">
         <v>144</v>
       </c>
-      <c r="G220" s="33"/>
-      <c r="H220" s="131"/>
-      <c r="I220" s="43" t="s">
+      <c r="G318" s="33"/>
+      <c r="H318" s="131"/>
+      <c r="I318" s="43" t="s">
         <v>1878</v>
       </c>
-      <c r="J220" s="27"/>
-      <c r="K220" s="34"/>
-      <c r="L220" s="39"/>
-      <c r="M220" s="34"/>
-    </row>
-    <row r="221" spans="1:13">
-      <c r="G221" s="33"/>
-      <c r="H221" s="38"/>
-      <c r="I221" s="33"/>
-      <c r="J221" s="27"/>
-      <c r="K221" s="34"/>
-      <c r="L221" s="39"/>
-      <c r="M221" s="34"/>
-    </row>
-    <row r="222" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A222" t="s">
+      <c r="J318" s="27"/>
+      <c r="K318" s="34"/>
+      <c r="L318" s="39"/>
+      <c r="M318" s="34"/>
+    </row>
+    <row r="319" spans="1:13">
+      <c r="G319" s="33"/>
+      <c r="H319" s="38"/>
+      <c r="I319" s="33"/>
+      <c r="J319" s="27"/>
+      <c r="K319" s="34"/>
+      <c r="L319" s="39"/>
+      <c r="M319" s="34"/>
+    </row>
+    <row r="320" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A320" t="s">
         <v>1871</v>
       </c>
-      <c r="G222" s="33"/>
-      <c r="H222" s="38"/>
-      <c r="I222" s="35"/>
-      <c r="J222" s="36"/>
-      <c r="K222" s="37"/>
-      <c r="L222" s="39"/>
-      <c r="M222" s="34"/>
-    </row>
-    <row r="223" spans="1:13">
-      <c r="B223" t="s">
+      <c r="G320" s="33"/>
+      <c r="H320" s="38"/>
+      <c r="I320" s="35"/>
+      <c r="J320" s="36"/>
+      <c r="K320" s="37"/>
+      <c r="L320" s="39"/>
+      <c r="M320" s="34"/>
+    </row>
+    <row r="321" spans="1:13">
+      <c r="B321" t="s">
         <v>1872</v>
       </c>
-      <c r="G223" s="33"/>
-      <c r="H223" s="38"/>
-      <c r="I223" s="39"/>
-      <c r="J223" s="39"/>
-      <c r="K223" s="39"/>
-      <c r="L223" s="39"/>
-      <c r="M223" s="34"/>
-    </row>
-    <row r="224" spans="1:13">
-      <c r="B224" t="s">
+      <c r="G321" s="33"/>
+      <c r="H321" s="38"/>
+      <c r="I321" s="39"/>
+      <c r="J321" s="39"/>
+      <c r="K321" s="39"/>
+      <c r="L321" s="39"/>
+      <c r="M321" s="34"/>
+    </row>
+    <row r="322" spans="1:13">
+      <c r="B322" t="s">
         <v>1873</v>
       </c>
-      <c r="G224" s="33"/>
-      <c r="H224" s="38"/>
-      <c r="I224" s="27"/>
-      <c r="J224" s="27"/>
-      <c r="K224" s="27"/>
-      <c r="L224" s="27"/>
-      <c r="M224" s="34"/>
-    </row>
-    <row r="225" spans="1:13">
-      <c r="C225" t="s">
+      <c r="G322" s="33"/>
+      <c r="H322" s="38"/>
+      <c r="I322" s="27"/>
+      <c r="J322" s="27"/>
+      <c r="K322" s="27"/>
+      <c r="L322" s="27"/>
+      <c r="M322" s="34"/>
+    </row>
+    <row r="323" spans="1:13">
+      <c r="C323" t="s">
         <v>1874</v>
       </c>
-      <c r="G225" s="33"/>
-      <c r="H225" s="27" t="s">
+      <c r="G323" s="33"/>
+      <c r="H323" s="27" t="s">
         <v>1881</v>
       </c>
-      <c r="I225" s="27"/>
-      <c r="J225" s="27"/>
-      <c r="K225" s="27"/>
-      <c r="L225" s="27"/>
-      <c r="M225" s="34"/>
-    </row>
-    <row r="226" spans="1:13">
-      <c r="B226" t="s">
+      <c r="I323" s="27"/>
+      <c r="J323" s="27"/>
+      <c r="K323" s="27"/>
+      <c r="L323" s="27"/>
+      <c r="M323" s="34"/>
+    </row>
+    <row r="324" spans="1:13">
+      <c r="B324" t="s">
         <v>144</v>
       </c>
-      <c r="G226" s="33"/>
-      <c r="H226" s="27"/>
-      <c r="I226" s="27"/>
-      <c r="J226" s="27"/>
-      <c r="K226" s="27"/>
-      <c r="L226" s="27"/>
-      <c r="M226" s="34"/>
-    </row>
-    <row r="227" spans="1:13">
-      <c r="A227" t="s">
+      <c r="G324" s="33"/>
+      <c r="H324" s="27"/>
+      <c r="I324" s="27"/>
+      <c r="J324" s="27"/>
+      <c r="K324" s="27"/>
+      <c r="L324" s="27"/>
+      <c r="M324" s="34"/>
+    </row>
+    <row r="325" spans="1:13">
+      <c r="A325" t="s">
         <v>144</v>
       </c>
-      <c r="G227" s="33"/>
-      <c r="H227" s="27"/>
-      <c r="I227" s="27"/>
-      <c r="J227" s="27"/>
-      <c r="K227" s="27"/>
-      <c r="L227" s="27"/>
-      <c r="M227" s="34"/>
-    </row>
-    <row r="228" spans="1:13" ht="15.75" thickBot="1">
-      <c r="G228" s="35"/>
-      <c r="H228" s="36"/>
-      <c r="I228" s="36"/>
-      <c r="J228" s="36"/>
-      <c r="K228" s="36"/>
-      <c r="L228" s="36"/>
-      <c r="M228" s="37"/>
-    </row>
-    <row r="229" spans="1:13">
-      <c r="A229" s="165" t="s">
+      <c r="G325" s="33"/>
+      <c r="H325" s="27"/>
+      <c r="I325" s="27"/>
+      <c r="J325" s="27"/>
+      <c r="K325" s="27"/>
+      <c r="L325" s="27"/>
+      <c r="M325" s="34"/>
+    </row>
+    <row r="326" spans="1:13" ht="15.75" thickBot="1">
+      <c r="G326" s="35"/>
+      <c r="H326" s="36"/>
+      <c r="I326" s="36"/>
+      <c r="J326" s="36"/>
+      <c r="K326" s="36"/>
+      <c r="L326" s="36"/>
+      <c r="M326" s="37"/>
+    </row>
+    <row r="327" spans="1:13">
+      <c r="A327" s="165" t="s">
         <v>1875</v>
       </c>
-      <c r="B229" s="29"/>
-      <c r="C229" s="29"/>
+      <c r="B327" s="29"/>
+      <c r="C327" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -51354,7 +51711,7 @@
   <dimension ref="A1:V411"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:P9"/>
+      <selection activeCell="N9" sqref="N9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
access privilege and abstract
</commit_message>
<xml_diff>
--- a/java_latest_st.xlsx
+++ b/java_latest_st.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="8" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="7305" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="references-latest" sheetId="28" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6306" uniqueCount="3288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6303" uniqueCount="3290">
   <si>
     <t>USER</t>
   </si>
@@ -9154,15 +9154,6 @@
     <t>Iphone6 &gt;</t>
   </si>
   <si>
-    <t>Iphone i1=new Iphone();</t>
-  </si>
-  <si>
-    <t>Iphone i2=new Iphone6();</t>
-  </si>
-  <si>
-    <t>Iphone i3=new IphoneX();</t>
-  </si>
-  <si>
     <t>Phone Calls</t>
   </si>
   <si>
@@ -9238,15 +9229,6 @@
     <t>cust2</t>
   </si>
   <si>
-    <t>static String bankName="Chase";</t>
-  </si>
-  <si>
-    <t>not shared</t>
-  </si>
-  <si>
-    <t>shared</t>
-  </si>
-  <si>
     <t>cust1.bankName="abcd";</t>
   </si>
   <si>
@@ -9256,13 +9238,6 @@
     <t>sysout( cust2.bankname);</t>
   </si>
   <si>
-    <t>bankName
-abcd</t>
-  </si>
-  <si>
-    <t>instance</t>
-  </si>
-  <si>
     <t>cust1.name="mike";</t>
   </si>
   <si>
@@ -10169,7 +10144,37 @@
     <t>inherit father and mother</t>
   </si>
   <si>
-    <t>confusion/ambiguity</t>
+    <t>Iphone i=new IphoneX();</t>
+  </si>
+  <si>
+    <t>new Iphonex();</t>
+  </si>
+  <si>
+    <t>Typecasting = unlock the disabled/hidden feature underneath</t>
+  </si>
+  <si>
+    <t>(IphoneX) I ).faceRecog();</t>
+  </si>
+  <si>
+    <t>Interface parent</t>
+  </si>
+  <si>
+    <t>Liberal</t>
+  </si>
+  <si>
+    <t>public default void occupation(){</t>
+  </si>
+  <si>
+    <t>sysout(it);</t>
+  </si>
+  <si>
+    <t>sysout(doctor);</t>
+  </si>
+  <si>
+    <t>String bankName="Chase";</t>
+  </si>
+  <si>
+    <t>Chase</t>
   </si>
 </sst>
 </file>
@@ -10763,7 +10768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="351">
+  <cellXfs count="350">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -11469,15 +11474,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -11490,6 +11486,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11805,13 +11807,13 @@
         <v>1904</v>
       </c>
       <c r="E1" t="s">
-        <v>3233</v>
+        <v>3225</v>
       </c>
       <c r="I1" s="56" t="s">
-        <v>3239</v>
+        <v>3231</v>
       </c>
       <c r="K1" t="s">
-        <v>3240</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1">
@@ -11895,7 +11897,7 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="A6" t="s">
-        <v>3237</v>
+        <v>3229</v>
       </c>
       <c r="E6" s="33"/>
       <c r="F6" s="27"/>
@@ -11912,7 +11914,7 @@
         <v>1512</v>
       </c>
       <c r="D7" t="s">
-        <v>3236</v>
+        <v>3228</v>
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="27"/>
@@ -11982,7 +11984,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1">
       <c r="A11" t="s">
-        <v>3232</v>
+        <v>3224</v>
       </c>
       <c r="E11" s="179" t="s">
         <v>178</v>
@@ -12020,7 +12022,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
       <c r="A13" t="s">
-        <v>3238</v>
+        <v>3230</v>
       </c>
       <c r="E13" s="205"/>
       <c r="F13" s="174"/>
@@ -12038,7 +12040,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1">
       <c r="A14" t="s">
-        <v>3231</v>
+        <v>3223</v>
       </c>
       <c r="E14" s="205"/>
       <c r="F14" s="174"/>
@@ -12086,7 +12088,7 @@
         <v>2764</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>3234</v>
+        <v>3226</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
@@ -12111,7 +12113,7 @@
         <v>192</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>3235</v>
+        <v>3227</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
@@ -19420,7 +19422,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
       <c r="A1" s="96" t="s">
-        <v>3258</v>
+        <v>3250</v>
       </c>
       <c r="B1" s="96"/>
       <c r="C1" s="96"/>
@@ -19440,7 +19442,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1">
       <c r="A2" s="96" t="s">
-        <v>3259</v>
+        <v>3251</v>
       </c>
       <c r="B2" s="96"/>
       <c r="C2" s="96"/>
@@ -19812,7 +19814,7 @@
       <c r="E18" s="65"/>
       <c r="F18" s="125"/>
       <c r="G18" s="147" t="s">
-        <v>3260</v>
+        <v>3252</v>
       </c>
       <c r="H18" s="149" t="s">
         <v>1657</v>
@@ -19842,7 +19844,7 @@
       </c>
       <c r="F19" s="96"/>
       <c r="G19" s="146" t="s">
-        <v>3261</v>
+        <v>3253</v>
       </c>
       <c r="H19" s="149"/>
       <c r="I19" s="288"/>
@@ -19869,7 +19871,7 @@
         <v>584</v>
       </c>
       <c r="F20" s="288" t="s">
-        <v>3262</v>
+        <v>3254</v>
       </c>
       <c r="G20" s="57"/>
       <c r="H20" s="64" t="s">
@@ -20749,7 +20751,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" s="165" t="s">
-        <v>3263</v>
+        <v>3255</v>
       </c>
       <c r="B1" s="165"/>
       <c r="E1" s="78" t="s">
@@ -20832,7 +20834,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1">
       <c r="B5" t="s">
-        <v>3264</v>
+        <v>3256</v>
       </c>
       <c r="E5" s="50"/>
       <c r="F5" s="51"/>
@@ -20862,7 +20864,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="C7" t="s">
-        <v>3265</v>
+        <v>3257</v>
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="27"/>
@@ -20940,7 +20942,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1">
       <c r="A12" t="s">
-        <v>3266</v>
+        <v>3258</v>
       </c>
       <c r="E12" s="33"/>
       <c r="F12" s="27"/>
@@ -20958,7 +20960,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>3267</v>
+        <v>3259</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="27"/>
@@ -20972,7 +20974,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>3268</v>
+        <v>3260</v>
       </c>
       <c r="E14" s="33"/>
       <c r="F14" s="27"/>
@@ -20986,7 +20988,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>3269</v>
+        <v>3261</v>
       </c>
       <c r="E15" s="33"/>
       <c r="F15" s="27"/>
@@ -21043,7 +21045,7 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" thickBot="1">
       <c r="B22" t="s">
-        <v>3270</v>
+        <v>3262</v>
       </c>
       <c r="F22" s="78" t="s">
         <v>1620</v>
@@ -21063,7 +21065,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="B23" t="s">
-        <v>3271</v>
+        <v>3263</v>
       </c>
       <c r="F23" s="33" t="s">
         <v>1939</v>
@@ -21085,7 +21087,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="B24" t="s">
-        <v>3272</v>
+        <v>3264</v>
       </c>
       <c r="F24" s="33" t="s">
         <v>1940</v>
@@ -21130,7 +21132,7 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1">
       <c r="B26" t="s">
-        <v>3273</v>
+        <v>3265</v>
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="27"/>
@@ -21139,7 +21141,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="53"/>
       <c r="L26" s="54" t="s">
-        <v>3280</v>
+        <v>3272</v>
       </c>
       <c r="M26" s="55" t="s">
         <v>2050</v>
@@ -21153,7 +21155,7 @@
         <v>2053</v>
       </c>
       <c r="D27" t="s">
-        <v>3281</v>
+        <v>3273</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="27"/>
@@ -21185,7 +21187,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="B29" t="s">
-        <v>3274</v>
+        <v>3266</v>
       </c>
       <c r="F29" s="33"/>
       <c r="G29" s="27"/>
@@ -21208,7 +21210,7 @@
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>3283</v>
+        <v>3275</v>
       </c>
       <c r="J30" s="27"/>
       <c r="K30" s="50"/>
@@ -21229,7 +21231,7 @@
         <v>2059</v>
       </c>
       <c r="G31" t="s">
-        <v>3284</v>
+        <v>3276</v>
       </c>
       <c r="J31" s="27"/>
       <c r="K31" s="50"/>
@@ -21247,15 +21249,15 @@
         <v>144</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>3282</v>
+        <v>3274</v>
       </c>
       <c r="G32" t="s">
-        <v>3285</v>
+        <v>3277</v>
       </c>
       <c r="J32" s="27"/>
       <c r="K32" s="53"/>
       <c r="L32" s="54" t="s">
-        <v>3280</v>
+        <v>3272</v>
       </c>
       <c r="M32" s="55" t="s">
         <v>2050</v>
@@ -21265,7 +21267,7 @@
     </row>
     <row r="33" spans="1:15">
       <c r="B33" t="s">
-        <v>3275</v>
+        <v>3267</v>
       </c>
       <c r="F33" s="33"/>
       <c r="G33" s="27"/>
@@ -21312,7 +21314,7 @@
     </row>
     <row r="36" spans="1:15">
       <c r="C36" t="s">
-        <v>3276</v>
+        <v>3268</v>
       </c>
       <c r="F36" s="33"/>
       <c r="G36" s="27"/>
@@ -21356,17 +21358,17 @@
       <c r="J38" s="27"/>
       <c r="K38" s="53"/>
       <c r="L38" s="54" t="s">
-        <v>3280</v>
+        <v>3272</v>
       </c>
       <c r="M38" s="55" t="s">
-        <v>3282</v>
+        <v>3274</v>
       </c>
       <c r="N38" s="27"/>
       <c r="O38" s="34"/>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" t="s">
-        <v>3277</v>
+        <v>3269</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="27"/>
@@ -21381,7 +21383,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>3278</v>
+        <v>3270</v>
       </c>
       <c r="F40" s="33"/>
       <c r="G40" s="27"/>
@@ -21396,7 +21398,7 @@
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1">
       <c r="A41" t="s">
-        <v>3279</v>
+        <v>3271</v>
       </c>
       <c r="F41" s="35"/>
       <c r="G41" s="36"/>
@@ -22986,8 +22988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23003,19 +23005,9 @@
         <v>760</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
-      <c r="H4" t="s">
-        <v>2949</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
-      <c r="H5" t="s">
-        <v>2950</v>
-      </c>
-    </row>
     <row r="6" spans="2:13">
       <c r="H6" s="56" t="s">
-        <v>2951</v>
+        <v>3279</v>
       </c>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
@@ -23074,13 +23066,13 @@
       <c r="C13" s="27"/>
       <c r="D13" s="34"/>
       <c r="E13" t="s">
-        <v>2955</v>
+        <v>2952</v>
       </c>
       <c r="F13" s="33"/>
       <c r="G13" s="27"/>
       <c r="H13" s="34"/>
       <c r="J13" s="289" t="s">
-        <v>2956</v>
+        <v>2953</v>
       </c>
       <c r="K13" s="33"/>
       <c r="L13" s="27"/>
@@ -23088,25 +23080,25 @@
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="33" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="34" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="34" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>2952</v>
+        <v>2949</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="34" t="s">
-        <v>2953</v>
+        <v>2950</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -23123,17 +23115,17 @@
     <row r="16" spans="2:13">
       <c r="B16" s="33"/>
       <c r="C16" s="27" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="D16" s="34"/>
       <c r="F16" s="33"/>
       <c r="G16" s="27" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="H16" s="34"/>
       <c r="K16" s="33"/>
       <c r="L16" s="27" t="s">
-        <v>2954</v>
+        <v>2951</v>
       </c>
       <c r="M16" s="34"/>
     </row>
@@ -23167,6 +23159,19 @@
         <v>760</v>
       </c>
     </row>
+    <row r="20" spans="2:13">
+      <c r="K20" t="s">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="F21" t="s">
+        <v>3280</v>
+      </c>
+      <c r="K21" t="s">
+        <v>3282</v>
+      </c>
+    </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>2063</v>
@@ -23197,7 +23202,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="49" spans="2:22">
+    <row r="49" spans="1:22">
       <c r="E49" s="30"/>
       <c r="F49" s="31"/>
       <c r="G49" s="32"/>
@@ -23205,34 +23210,34 @@
       <c r="L49" s="31"/>
       <c r="M49" s="32"/>
     </row>
-    <row r="50" spans="2:22">
+    <row r="50" spans="1:22">
       <c r="E50" s="33" t="s">
-        <v>725</v>
+        <v>3285</v>
       </c>
       <c r="F50" s="27"/>
       <c r="G50" s="34"/>
       <c r="K50" s="33" t="s">
-        <v>725</v>
+        <v>3285</v>
       </c>
       <c r="L50" s="27"/>
       <c r="M50" s="34"/>
     </row>
-    <row r="51" spans="2:22">
+    <row r="51" spans="1:22">
       <c r="B51" t="s">
         <v>2945</v>
       </c>
       <c r="E51" s="33"/>
       <c r="F51" s="27" t="s">
-        <v>727</v>
+        <v>3286</v>
       </c>
       <c r="G51" s="34"/>
       <c r="K51" s="33"/>
       <c r="L51" s="27" t="s">
-        <v>726</v>
+        <v>3287</v>
       </c>
       <c r="M51" s="34"/>
     </row>
-    <row r="52" spans="2:22" ht="15.75" thickBot="1">
+    <row r="52" spans="1:22" ht="15.75" thickBot="1">
       <c r="E52" s="35" t="s">
         <v>144</v>
       </c>
@@ -23244,7 +23249,7 @@
       <c r="L52" s="36"/>
       <c r="M52" s="37"/>
     </row>
-    <row r="53" spans="2:22">
+    <row r="53" spans="1:22">
       <c r="B53" t="s">
         <v>2454</v>
       </c>
@@ -23252,12 +23257,12 @@
         <v>733</v>
       </c>
     </row>
-    <row r="54" spans="2:22">
+    <row r="54" spans="1:22">
       <c r="P54" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="55" spans="2:22" ht="15.75" thickBot="1">
+    <row r="55" spans="1:22" ht="15.75" thickBot="1">
       <c r="B55" t="s">
         <v>728</v>
       </c>
@@ -23265,35 +23270,32 @@
         <v>728</v>
       </c>
       <c r="I55" t="s">
-        <v>3286</v>
-      </c>
-    </row>
-    <row r="56" spans="2:22">
+        <v>3278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="H56" s="30"/>
       <c r="I56" s="31"/>
       <c r="J56" s="32"/>
     </row>
-    <row r="57" spans="2:22">
+    <row r="57" spans="1:22">
       <c r="H57" s="33"/>
-      <c r="I57" t="s">
-        <v>729</v>
-      </c>
       <c r="J57" s="34"/>
       <c r="P57" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="58" spans="2:22">
+    <row r="58" spans="1:22">
+      <c r="A58" t="s">
+        <v>3283</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3284</v>
+      </c>
       <c r="H58" s="33"/>
-      <c r="I58" t="s">
-        <v>730</v>
-      </c>
       <c r="J58" s="34"/>
-      <c r="K58" t="s">
-        <v>3287</v>
-      </c>
-    </row>
-    <row r="59" spans="2:22">
+    </row>
+    <row r="59" spans="1:22">
       <c r="H59" s="33"/>
       <c r="I59" s="27"/>
       <c r="J59" s="34"/>
@@ -23304,12 +23306,12 @@
         <v>739</v>
       </c>
     </row>
-    <row r="60" spans="2:22">
+    <row r="60" spans="1:22">
       <c r="H60" s="33"/>
       <c r="I60" s="27"/>
       <c r="J60" s="34"/>
     </row>
-    <row r="61" spans="2:22" ht="15.75" thickBot="1">
+    <row r="61" spans="1:22" ht="15.75" thickBot="1">
       <c r="H61" s="35"/>
       <c r="I61" s="36"/>
       <c r="J61" s="37"/>
@@ -23323,7 +23325,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="63" spans="2:22">
+    <row r="63" spans="1:22">
       <c r="B63" t="s">
         <v>731</v>
       </c>
@@ -23508,16 +23510,16 @@
     </row>
     <row r="78" spans="2:21">
       <c r="B78" t="s">
-        <v>2957</v>
+        <v>2954</v>
       </c>
       <c r="C78" t="s">
         <v>2790</v>
       </c>
       <c r="D78" t="s">
-        <v>2958</v>
+        <v>2955</v>
       </c>
       <c r="E78" t="s">
-        <v>2959</v>
+        <v>2956</v>
       </c>
       <c r="F78" t="s">
         <v>223</v>
@@ -23534,7 +23536,7 @@
     </row>
     <row r="79" spans="2:21">
       <c r="F79" t="s">
-        <v>2960</v>
+        <v>2957</v>
       </c>
       <c r="I79" t="s">
         <v>144</v>
@@ -23545,16 +23547,16 @@
     </row>
     <row r="80" spans="2:21">
       <c r="B80" t="s">
-        <v>2957</v>
+        <v>2954</v>
       </c>
       <c r="C80" t="s">
         <v>2790</v>
       </c>
       <c r="D80" t="s">
-        <v>2958</v>
+        <v>2955</v>
       </c>
       <c r="E80" t="s">
-        <v>2958</v>
+        <v>2955</v>
       </c>
       <c r="N80" t="s">
         <v>144</v>
@@ -23562,12 +23564,12 @@
     </row>
     <row r="81" spans="2:10">
       <c r="F81" t="s">
-        <v>2961</v>
+        <v>2958</v>
       </c>
     </row>
     <row r="82" spans="2:10">
       <c r="F82" t="s">
-        <v>2962</v>
+        <v>2959</v>
       </c>
       <c r="J82" t="s">
         <v>747</v>
@@ -23575,31 +23577,31 @@
     </row>
     <row r="83" spans="2:10">
       <c r="B83" t="s">
-        <v>2957</v>
+        <v>2954</v>
       </c>
       <c r="C83" t="s">
         <v>2790</v>
       </c>
       <c r="D83" t="s">
-        <v>2966</v>
+        <v>2963</v>
       </c>
       <c r="E83" t="s">
-        <v>2963</v>
+        <v>2960</v>
       </c>
     </row>
     <row r="84" spans="2:10">
       <c r="F84" t="s">
-        <v>2964</v>
+        <v>2961</v>
       </c>
     </row>
     <row r="85" spans="2:10">
       <c r="F85" t="s">
-        <v>2965</v>
+        <v>2962</v>
       </c>
     </row>
     <row r="87" spans="2:10">
       <c r="B87" t="s">
-        <v>2967</v>
+        <v>2964</v>
       </c>
       <c r="J87" t="s">
         <v>750</v>
@@ -25999,10 +26001,10 @@
       <c r="M5" s="2"/>
       <c r="N5" s="3"/>
       <c r="P5" t="s">
-        <v>3164</v>
+        <v>3156</v>
       </c>
       <c r="Q5" t="s">
-        <v>3165</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1">
@@ -26025,7 +26027,7 @@
         <v>411</v>
       </c>
       <c r="Q6" t="s">
-        <v>3163</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1">
@@ -26042,10 +26044,10 @@
       <c r="M7" s="5"/>
       <c r="N7" s="6"/>
       <c r="P7" t="s">
-        <v>3161</v>
+        <v>3153</v>
       </c>
       <c r="Q7" t="s">
-        <v>3162</v>
+        <v>3154</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -26065,15 +26067,15 @@
       </c>
       <c r="N8" s="337"/>
       <c r="P8" t="s">
-        <v>3147</v>
+        <v>3139</v>
       </c>
       <c r="Q8" s="142" t="s">
-        <v>3160</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="B9" t="s">
-        <v>3140</v>
+        <v>3132</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="253"/>
@@ -26102,10 +26104,10 @@
       <c r="M10" s="253"/>
       <c r="N10" s="253"/>
       <c r="P10" t="s">
-        <v>3145</v>
+        <v>3137</v>
       </c>
       <c r="Q10" s="142" t="s">
-        <v>3146</v>
+        <v>3138</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -26122,7 +26124,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="B12" t="s">
-        <v>3141</v>
+        <v>3133</v>
       </c>
       <c r="F12" s="327" t="s">
         <v>2659</v>
@@ -26148,7 +26150,7 @@
       <c r="M13" s="330"/>
       <c r="N13" s="330"/>
       <c r="P13" t="s">
-        <v>3148</v>
+        <v>3140</v>
       </c>
       <c r="Q13">
         <v>10</v>
@@ -26192,7 +26194,7 @@
       <c r="M15" s="11"/>
       <c r="N15" s="12"/>
       <c r="P15" t="s">
-        <v>3142</v>
+        <v>3134</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -26232,7 +26234,7 @@
       <c r="M17" s="136"/>
       <c r="N17" s="18"/>
       <c r="Q17" t="s">
-        <v>3143</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1">
@@ -26272,7 +26274,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="18"/>
       <c r="J20" s="13" t="s">
-        <v>3181</v>
+        <v>3173</v>
       </c>
       <c r="K20" s="15" t="s">
         <v>524</v>
@@ -26283,7 +26285,7 @@
       </c>
       <c r="N20" s="18"/>
       <c r="Q20" s="142" t="s">
-        <v>3144</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -26327,7 +26329,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="18"/>
       <c r="J23" s="13" t="s">
-        <v>3181</v>
+        <v>3173</v>
       </c>
       <c r="K23" s="15" t="s">
         <v>412</v>
@@ -26360,7 +26362,7 @@
       <c r="I25" s="22"/>
       <c r="J25" s="317"/>
       <c r="K25" s="22" t="s">
-        <v>3182</v>
+        <v>3174</v>
       </c>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
@@ -26368,43 +26370,43 @@
     </row>
     <row r="27" spans="1:17">
       <c r="H27" t="s">
-        <v>3192</v>
+        <v>3184</v>
       </c>
       <c r="O27" t="s">
-        <v>3148</v>
+        <v>3140</v>
       </c>
       <c r="P27" t="s">
-        <v>3154</v>
+        <v>3146</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="O28" t="s">
-        <v>3155</v>
+        <v>3147</v>
       </c>
       <c r="P28" t="s">
-        <v>3150</v>
+        <v>3142</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1">
       <c r="O29" t="s">
-        <v>3158</v>
+        <v>3150</v>
       </c>
       <c r="P29" t="s">
-        <v>3151</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="G30" s="26"/>
       <c r="O30" t="s">
-        <v>3159</v>
+        <v>3151</v>
       </c>
       <c r="P30" t="s">
-        <v>3152</v>
+        <v>3144</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="G31" s="326" t="s">
-        <v>3149</v>
+        <v>3141</v>
       </c>
       <c r="H31" s="326"/>
       <c r="I31" s="326"/>
@@ -26414,7 +26416,7 @@
       <c r="M31" s="326"/>
       <c r="N31" s="326"/>
       <c r="P31" t="s">
-        <v>3153</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -26592,7 +26594,7 @@
         <v>1</v>
       </c>
       <c r="O37" s="57" t="s">
-        <v>3257</v>
+        <v>3249</v>
       </c>
       <c r="P37" s="57">
         <v>15</v>
@@ -26688,7 +26690,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
       <c r="P42" t="s">
-        <v>3157</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="43" spans="1:17 16384:16384">
@@ -26707,7 +26709,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
       <c r="P43" t="s">
-        <v>3156</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="44" spans="1:17 16384:16384">
@@ -27220,7 +27222,7 @@
         <v>47</v>
       </c>
       <c r="J126" t="s">
-        <v>3166</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="129" spans="1:18">
@@ -27228,13 +27230,13 @@
         <v>1819</v>
       </c>
       <c r="J129" t="s">
-        <v>3166</v>
+        <v>3158</v>
       </c>
     </row>
     <row r="132" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="133" spans="1:18">
       <c r="F133" s="30" t="s">
-        <v>3167</v>
+        <v>3159</v>
       </c>
       <c r="G133" s="31"/>
       <c r="H133" s="32"/>
@@ -27256,7 +27258,7 @@
         <v>2651</v>
       </c>
       <c r="G134" s="27" t="s">
-        <v>3177</v>
+        <v>3169</v>
       </c>
       <c r="H134" s="34"/>
       <c r="J134" s="33"/>
@@ -27264,21 +27266,21 @@
         <v>2214</v>
       </c>
       <c r="L134" s="27" t="s">
-        <v>3179</v>
+        <v>3171</v>
       </c>
       <c r="M134" s="34"/>
       <c r="O134" s="33" t="s">
         <v>1583</v>
       </c>
       <c r="P134" s="27" t="s">
-        <v>3180</v>
+        <v>3172</v>
       </c>
       <c r="Q134" s="27"/>
       <c r="R134" s="34"/>
     </row>
     <row r="135" spans="1:18">
       <c r="A135" t="s">
-        <v>3183</v>
+        <v>3175</v>
       </c>
       <c r="F135" s="33"/>
       <c r="G135" s="27"/>
@@ -27310,13 +27312,13 @@
     </row>
     <row r="137" spans="1:18">
       <c r="A137" t="s">
-        <v>3184</v>
+        <v>3176</v>
       </c>
       <c r="E137" t="s">
-        <v>3169</v>
+        <v>3161</v>
       </c>
       <c r="F137" s="33" t="s">
-        <v>3168</v>
+        <v>3160</v>
       </c>
       <c r="G137" s="27"/>
       <c r="H137" s="34" t="s">
@@ -27387,30 +27389,30 @@
     </row>
     <row r="142" spans="1:18">
       <c r="E142" t="s">
-        <v>3172</v>
+        <v>3164</v>
       </c>
       <c r="F142" s="33" t="s">
-        <v>3170</v>
+        <v>3162</v>
       </c>
       <c r="G142" s="27"/>
       <c r="H142" s="34" t="s">
         <v>1603</v>
       </c>
       <c r="J142" s="33" t="s">
-        <v>3172</v>
+        <v>3164</v>
       </c>
       <c r="K142" s="27" t="s">
-        <v>3170</v>
+        <v>3162</v>
       </c>
       <c r="L142" s="27"/>
       <c r="M142" s="34" t="s">
         <v>1603</v>
       </c>
       <c r="O142" s="33" t="s">
-        <v>3172</v>
+        <v>3164</v>
       </c>
       <c r="P142" s="27" t="s">
-        <v>3170</v>
+        <v>3162</v>
       </c>
       <c r="Q142" s="27"/>
       <c r="R142" s="34" t="s">
@@ -27419,45 +27421,45 @@
     </row>
     <row r="143" spans="1:18">
       <c r="E143" t="s">
-        <v>3173</v>
+        <v>3165</v>
       </c>
       <c r="F143" s="33" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="G143" s="27"/>
       <c r="H143" s="34"/>
       <c r="J143" s="33" t="s">
-        <v>3173</v>
+        <v>3165</v>
       </c>
       <c r="K143" s="27" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="L143" s="27"/>
       <c r="M143" s="34"/>
       <c r="O143" s="33" t="s">
-        <v>3173</v>
+        <v>3165</v>
       </c>
       <c r="P143" s="27" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="Q143" s="27"/>
       <c r="R143" s="34"/>
     </row>
     <row r="144" spans="1:18">
       <c r="E144" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="F144" s="33"/>
       <c r="G144" s="27"/>
       <c r="H144" s="34"/>
       <c r="J144" s="33" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="K144" s="27"/>
       <c r="L144" s="27"/>
       <c r="M144" s="34"/>
       <c r="O144" s="33" t="s">
-        <v>3171</v>
+        <v>3163</v>
       </c>
       <c r="P144" s="27"/>
       <c r="Q144" s="27"/>
@@ -27478,19 +27480,19 @@
     </row>
     <row r="146" spans="5:18">
       <c r="F146" s="80" t="s">
-        <v>3166</v>
+        <v>3158</v>
       </c>
       <c r="G146" s="27"/>
       <c r="H146" s="34"/>
       <c r="J146" s="33"/>
       <c r="K146" s="39" t="s">
-        <v>3186</v>
+        <v>3178</v>
       </c>
       <c r="L146" s="27"/>
       <c r="M146" s="34"/>
       <c r="O146" s="33"/>
       <c r="P146" s="39" t="s">
-        <v>3186</v>
+        <v>3178</v>
       </c>
       <c r="Q146" s="27"/>
       <c r="R146" s="34"/>
@@ -27510,26 +27512,26 @@
     </row>
     <row r="148" spans="5:18">
       <c r="E148" t="s">
-        <v>3176</v>
+        <v>3168</v>
       </c>
       <c r="F148" s="33" t="s">
-        <v>3175</v>
+        <v>3167</v>
       </c>
       <c r="G148" s="27"/>
       <c r="H148" s="34"/>
       <c r="J148" s="33" t="s">
-        <v>3176</v>
+        <v>3168</v>
       </c>
       <c r="K148" s="27" t="s">
-        <v>3175</v>
+        <v>3167</v>
       </c>
       <c r="L148" s="27"/>
       <c r="M148" s="34"/>
       <c r="O148" s="33" t="s">
-        <v>3176</v>
+        <v>3168</v>
       </c>
       <c r="P148" s="27" t="s">
-        <v>3175</v>
+        <v>3167</v>
       </c>
       <c r="Q148" s="27"/>
       <c r="R148" s="34"/>
@@ -27562,19 +27564,19 @@
     </row>
     <row r="151" spans="5:18">
       <c r="F151" s="33" t="s">
-        <v>3174</v>
+        <v>3166</v>
       </c>
       <c r="G151" s="27"/>
       <c r="H151" s="34"/>
       <c r="J151" s="33"/>
       <c r="K151" s="27" t="s">
-        <v>3178</v>
+        <v>3170</v>
       </c>
       <c r="L151" s="27"/>
       <c r="M151" s="34"/>
       <c r="O151" s="33"/>
       <c r="P151" s="27" t="s">
-        <v>3185</v>
+        <v>3177</v>
       </c>
       <c r="Q151" s="27"/>
       <c r="R151" s="34"/>
@@ -27607,7 +27609,7 @@
     </row>
     <row r="160" spans="5:18">
       <c r="F160" t="s">
-        <v>3187</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="162" spans="9:12">
@@ -27620,18 +27622,18 @@
     </row>
     <row r="163" spans="9:12">
       <c r="I163" t="s">
-        <v>3190</v>
+        <v>3182</v>
       </c>
       <c r="L163" t="s">
-        <v>3191</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="164" spans="9:12">
       <c r="I164" t="s">
-        <v>3188</v>
+        <v>3180</v>
       </c>
       <c r="L164" t="s">
-        <v>3189</v>
+        <v>3181</v>
       </c>
     </row>
   </sheetData>
@@ -27655,8 +27657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R293"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:M6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27672,20 +27674,15 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1">
       <c r="A1" s="96" t="s">
-        <v>2968</v>
+        <v>2965</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="96" t="s">
-        <v>2979</v>
-      </c>
+      <c r="A2" s="96"/>
       <c r="B2" s="96" t="s">
-        <v>2977</v>
+        <v>3288</v>
       </c>
       <c r="C2" s="96"/>
-      <c r="E2" s="57" t="s">
-        <v>1003</v>
-      </c>
       <c r="G2" s="47"/>
       <c r="H2" s="48"/>
       <c r="I2" s="48"/>
@@ -27698,17 +27695,12 @@
       <c r="P2" s="48"/>
       <c r="Q2" s="49"/>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="96" t="s">
-        <v>2978</v>
-      </c>
+    <row r="3" spans="1:17" ht="15" customHeight="1">
+      <c r="A3" s="96"/>
       <c r="B3" s="96" t="s">
         <v>460</v>
       </c>
       <c r="C3" s="96"/>
-      <c r="E3" s="57" t="s">
-        <v>2984</v>
-      </c>
       <c r="G3" s="50"/>
       <c r="H3" s="51" t="s">
         <v>204</v>
@@ -27721,37 +27713,34 @@
         <v>413</v>
       </c>
       <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="343" t="s">
-        <v>2983</v>
-      </c>
+      <c r="M3" s="49"/>
+      <c r="N3" s="348"/>
       <c r="O3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="96" t="s">
-        <v>2978</v>
-      </c>
+      <c r="A4" s="96"/>
       <c r="B4" s="96" t="s">
-        <v>2969</v>
+        <v>2966</v>
       </c>
       <c r="C4" s="96"/>
-      <c r="E4" s="57" t="s">
-        <v>2984</v>
-      </c>
       <c r="G4" s="50"/>
       <c r="H4" s="51" t="s">
-        <v>2974</v>
+        <v>2971</v>
       </c>
       <c r="I4" s="51" t="s">
         <v>413</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="51"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="344"/>
+      <c r="L4" s="50" t="s">
+        <v>1728</v>
+      </c>
+      <c r="M4" s="52" t="s">
+        <v>3289</v>
+      </c>
+      <c r="N4" s="349"/>
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="52"/>
@@ -27759,12 +27748,12 @@
     <row r="5" spans="1:17">
       <c r="A5" s="96"/>
       <c r="B5" s="96" t="s">
-        <v>2970</v>
+        <v>2967</v>
       </c>
       <c r="C5" s="96"/>
       <c r="G5" s="50"/>
       <c r="H5" s="51" t="s">
-        <v>2976</v>
+        <v>2973</v>
       </c>
       <c r="I5" s="51" t="s">
         <v>1951</v>
@@ -27774,10 +27763,10 @@
       <c r="L5" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="51" t="s">
+      <c r="M5" s="52" t="s">
         <v>559</v>
       </c>
-      <c r="N5" s="344"/>
+      <c r="N5" s="349"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="52"/>
@@ -27794,12 +27783,12 @@
       <c r="J6" s="51"/>
       <c r="K6" s="51"/>
       <c r="L6" s="53" t="s">
-        <v>2975</v>
-      </c>
-      <c r="M6" s="54">
+        <v>2972</v>
+      </c>
+      <c r="M6" s="55">
         <v>12345</v>
       </c>
-      <c r="N6" s="344"/>
+      <c r="N6" s="349"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="52"/>
@@ -27808,7 +27797,7 @@
       <c r="A7" s="96"/>
       <c r="B7" s="96"/>
       <c r="C7" s="96" t="s">
-        <v>2971</v>
+        <v>2968</v>
       </c>
       <c r="G7" s="50"/>
       <c r="H7" s="51"/>
@@ -27817,7 +27806,7 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="344"/>
+      <c r="N7" s="349"/>
       <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="52"/>
@@ -27836,8 +27825,8 @@
         <v>1951</v>
       </c>
       <c r="L8" s="47"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="344"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="349"/>
       <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="52"/>
@@ -27853,9 +27842,13 @@
       <c r="I9" s="51"/>
       <c r="J9" s="51"/>
       <c r="K9" s="51"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="344"/>
+      <c r="L9" s="50" t="s">
+        <v>1728</v>
+      </c>
+      <c r="M9" s="52" t="s">
+        <v>3289</v>
+      </c>
+      <c r="N9" s="349"/>
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="52"/>
@@ -27869,17 +27862,17 @@
       <c r="L10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="M10" s="51" t="s">
+      <c r="M10" s="52" t="s">
         <v>524</v>
       </c>
-      <c r="N10" s="344"/>
+      <c r="N10" s="349"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1">
       <c r="C11" s="57" t="s">
-        <v>2972</v>
+        <v>2969</v>
       </c>
       <c r="G11" s="50"/>
       <c r="H11" s="51"/>
@@ -27887,19 +27880,19 @@
       <c r="J11" s="51"/>
       <c r="K11" s="51"/>
       <c r="L11" s="53" t="s">
-        <v>2975</v>
-      </c>
-      <c r="M11" s="54">
+        <v>2972</v>
+      </c>
+      <c r="M11" s="55">
         <v>12346</v>
       </c>
-      <c r="N11" s="345"/>
+      <c r="N11" s="349"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="52"/>
     </row>
     <row r="12" spans="1:17">
       <c r="C12" s="57" t="s">
-        <v>2973</v>
+        <v>2970</v>
       </c>
       <c r="G12" s="50"/>
       <c r="H12" s="51"/>
@@ -27915,7 +27908,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="B13" s="57" t="s">
-        <v>2980</v>
+        <v>2974</v>
       </c>
       <c r="G13" s="50"/>
       <c r="H13" s="51"/>
@@ -27931,7 +27924,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="B14" s="57" t="s">
-        <v>2981</v>
+        <v>2975</v>
       </c>
       <c r="D14" s="57" t="s">
         <v>2816</v>
@@ -27950,7 +27943,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="B15" s="57" t="s">
-        <v>2982</v>
+        <v>2976</v>
       </c>
       <c r="D15" s="57" t="s">
         <v>2816</v>
@@ -27982,7 +27975,7 @@
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="57" t="s">
-        <v>2985</v>
+        <v>2977</v>
       </c>
       <c r="G17" s="50"/>
       <c r="H17" s="51"/>
@@ -27998,7 +27991,7 @@
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="57" t="s">
-        <v>2986</v>
+        <v>2978</v>
       </c>
       <c r="D18" s="57" t="s">
         <v>559</v>
@@ -28017,7 +28010,7 @@
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="57" t="s">
-        <v>2987</v>
+        <v>2979</v>
       </c>
       <c r="D19" s="57" t="s">
         <v>524</v>
@@ -31208,9 +31201,6 @@
       <c r="Q293" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="N3:N11"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -31232,10 +31222,10 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>2988</v>
+        <v>2980</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>2992</v>
+        <v>2984</v>
       </c>
       <c r="H1" s="31" t="s">
         <v>413</v>
@@ -31250,10 +31240,10 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1">
       <c r="A2" t="s">
-        <v>2989</v>
+        <v>2981</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>2993</v>
+        <v>2985</v>
       </c>
       <c r="H2" s="27" t="s">
         <v>1951</v>
@@ -31270,10 +31260,10 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
       <c r="A3" t="s">
-        <v>2990</v>
+        <v>2982</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>2994</v>
+        <v>2986</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>2629</v>
@@ -31286,7 +31276,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="G4" s="33" t="s">
-        <v>2997</v>
+        <v>2989</v>
       </c>
       <c r="H4" s="38" t="s">
         <v>417</v>
@@ -31314,7 +31304,7 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1">
       <c r="G6" s="33" t="s">
-        <v>2995</v>
+        <v>2987</v>
       </c>
       <c r="H6" s="301">
         <v>0</v>
@@ -31329,7 +31319,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>2991</v>
+        <v>2983</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="301">
@@ -31347,10 +31337,10 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
       <c r="A8" t="s">
-        <v>2998</v>
+        <v>2990</v>
       </c>
       <c r="D8" t="s">
-        <v>3004</v>
+        <v>2996</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="301">
@@ -31370,7 +31360,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>2999</v>
+        <v>2991</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="301">
@@ -31386,7 +31376,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>3000</v>
+        <v>2992</v>
       </c>
       <c r="G10" s="33"/>
       <c r="H10" s="301">
@@ -31402,7 +31392,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>3001</v>
+        <v>2993</v>
       </c>
       <c r="G11" s="33"/>
       <c r="H11" s="27"/>
@@ -31414,7 +31404,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>2996</v>
+        <v>2988</v>
       </c>
       <c r="G12" s="33"/>
       <c r="H12" s="27"/>
@@ -31435,7 +31425,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="B14" t="s">
-        <v>3002</v>
+        <v>2994</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
@@ -31447,7 +31437,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" t="s">
-        <v>3003</v>
+        <v>2995</v>
       </c>
       <c r="G15" s="33"/>
       <c r="H15" s="27"/>
@@ -31486,7 +31476,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>3005</v>
+        <v>2997</v>
       </c>
       <c r="E22" t="s">
         <v>1914</v>
@@ -31494,7 +31484,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>3006</v>
+        <v>2998</v>
       </c>
       <c r="E23" s="57"/>
       <c r="F23" s="57">
@@ -31536,10 +31526,10 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>3007</v>
+        <v>2999</v>
       </c>
       <c r="D29" t="s">
-        <v>3014</v>
+        <v>3006</v>
       </c>
       <c r="E29" s="129">
         <v>0</v>
@@ -31548,7 +31538,7 @@
         <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>3015</v>
+        <v>3007</v>
       </c>
       <c r="I29" s="129">
         <v>0</v>
@@ -31559,7 +31549,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>3008</v>
+        <v>3000</v>
       </c>
       <c r="E30" s="129">
         <v>1</v>
@@ -31576,7 +31566,7 @@
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>3009</v>
+        <v>3001</v>
       </c>
       <c r="E31" s="129">
         <v>2</v>
@@ -31593,7 +31583,7 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>3010</v>
+        <v>3002</v>
       </c>
       <c r="E32" s="129">
         <v>3</v>
@@ -31610,7 +31600,7 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>3011</v>
+        <v>3003</v>
       </c>
       <c r="E33" s="129">
         <v>4</v>
@@ -31627,15 +31617,15 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>3012</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>3013</v>
+        <v>3005</v>
       </c>
       <c r="E35" t="s">
-        <v>3016</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1"/>
@@ -34276,7 +34266,7 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
       <c r="A4" t="s">
-        <v>3020</v>
+        <v>3012</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>549</v>
@@ -34294,7 +34284,7 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
       <c r="A5" t="s">
-        <v>3021</v>
+        <v>3013</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>550</v>
@@ -34334,7 +34324,7 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
       <c r="A7" t="s">
-        <v>3023</v>
+        <v>3015</v>
       </c>
       <c r="F7" s="50" t="s">
         <v>1140</v>
@@ -34369,10 +34359,10 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" t="s">
-        <v>3046</v>
+        <v>3038</v>
       </c>
       <c r="F9" s="50" t="s">
-        <v>3024</v>
+        <v>3016</v>
       </c>
       <c r="G9" s="38" t="s">
         <v>2767</v>
@@ -34435,7 +34425,7 @@
       <c r="J12" s="27"/>
       <c r="K12" s="33"/>
       <c r="L12" s="38" t="s">
-        <v>3028</v>
+        <v>3020</v>
       </c>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
@@ -34472,18 +34462,18 @@
     </row>
     <row r="17" spans="1:15">
       <c r="G17" t="s">
-        <v>3022</v>
+        <v>3014</v>
       </c>
       <c r="I17" t="s">
-        <v>3025</v>
+        <v>3017</v>
       </c>
       <c r="K17" t="s">
-        <v>3026</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="K18" s="56" t="s">
-        <v>3027</v>
+        <v>3019</v>
       </c>
       <c r="L18" s="56"/>
       <c r="M18" s="56"/>
@@ -34492,7 +34482,7 @@
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1">
       <c r="A20" t="s">
-        <v>3033</v>
+        <v>3025</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1">
@@ -34510,7 +34500,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>3029</v>
+        <v>3021</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="27"/>
@@ -34518,7 +34508,7 @@
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="303" t="s">
-        <v>3039</v>
+        <v>3031</v>
       </c>
       <c r="I22" s="31"/>
       <c r="J22" s="32"/>
@@ -34526,13 +34516,13 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>3032</v>
+        <v>3024</v>
       </c>
       <c r="C23" s="50" t="s">
         <v>549</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>3036</v>
+        <v>3028</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38"/>
@@ -34541,14 +34531,14 @@
         <v>1908</v>
       </c>
       <c r="I23" s="247" t="s">
-        <v>3034</v>
+        <v>3026</v>
       </c>
       <c r="J23" s="34"/>
       <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>3030</v>
+        <v>3022</v>
       </c>
       <c r="C24" s="38" t="s">
         <v>2168</v>
@@ -34570,7 +34560,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1">
       <c r="A25" t="s">
-        <v>3031</v>
+        <v>3023</v>
       </c>
       <c r="C25" s="50"/>
       <c r="D25" s="38"/>
@@ -34593,7 +34583,7 @@
         <v>413</v>
       </c>
       <c r="F26" s="307" t="s">
-        <v>3042</v>
+        <v>3034</v>
       </c>
       <c r="G26" s="27"/>
       <c r="H26" s="304" t="s">
@@ -34615,14 +34605,14 @@
         <v>2631</v>
       </c>
       <c r="I27" s="247" t="s">
-        <v>3040</v>
+        <v>3032</v>
       </c>
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
     </row>
     <row r="28" spans="1:15">
       <c r="A28" t="s">
-        <v>3044</v>
+        <v>3036</v>
       </c>
       <c r="C28" s="50"/>
       <c r="D28" s="38"/>
@@ -34630,27 +34620,27 @@
       <c r="F28" s="38"/>
       <c r="G28" s="27"/>
       <c r="H28" s="304" t="s">
-        <v>3035</v>
+        <v>3027</v>
       </c>
       <c r="I28" s="246" t="s">
-        <v>3041</v>
+        <v>3033</v>
       </c>
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
     </row>
     <row r="29" spans="1:15">
       <c r="A29" t="s">
-        <v>3045</v>
+        <v>3037</v>
       </c>
       <c r="C29" s="50"/>
       <c r="D29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="27"/>
       <c r="H29" s="304" t="s">
-        <v>3036</v>
+        <v>3028</v>
       </c>
       <c r="I29" s="247" t="s">
-        <v>3042</v>
+        <v>3034</v>
       </c>
       <c r="J29" s="34"/>
       <c r="K29" s="34"/>
@@ -34665,7 +34655,7 @@
       <c r="F30" s="38"/>
       <c r="G30" s="27"/>
       <c r="H30" s="304" t="s">
-        <v>3037</v>
+        <v>3029</v>
       </c>
       <c r="I30" s="247"/>
       <c r="J30" s="34"/>
@@ -34679,7 +34669,7 @@
       <c r="F31" s="38"/>
       <c r="G31" s="27"/>
       <c r="H31" s="304" t="s">
-        <v>3038</v>
+        <v>3030</v>
       </c>
       <c r="I31" s="246"/>
       <c r="J31" s="34"/>
@@ -34714,7 +34704,7 @@
     </row>
     <row r="36" spans="2:15">
       <c r="B36" t="s">
-        <v>3043</v>
+        <v>3035</v>
       </c>
     </row>
     <row r="37" spans="2:15">
@@ -39940,7 +39930,7 @@
     </row>
     <row r="333" spans="1:12">
       <c r="B333" t="s">
-        <v>3017</v>
+        <v>3009</v>
       </c>
       <c r="F333" s="33"/>
       <c r="G333" s="27" t="s">
@@ -40023,7 +40013,7 @@
     </row>
     <row r="340" spans="2:12">
       <c r="B340" t="s">
-        <v>3018</v>
+        <v>3010</v>
       </c>
       <c r="D340" t="s">
         <v>412</v>
@@ -40038,7 +40028,7 @@
     </row>
     <row r="341" spans="2:12">
       <c r="B341" t="s">
-        <v>3019</v>
+        <v>3011</v>
       </c>
       <c r="F341" s="33"/>
       <c r="G341" s="27"/>
@@ -40108,59 +40098,59 @@
     </row>
     <row r="4" spans="2:13">
       <c r="C4" t="s">
-        <v>3056</v>
+        <v>3048</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>3050</v>
+        <v>3042</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>3051</v>
+        <v>3043</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>3048</v>
+        <v>3040</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>3049</v>
+        <v>3041</v>
       </c>
       <c r="I4" t="s">
-        <v>3063</v>
+        <v>3055</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="C5" t="s">
-        <v>3057</v>
+        <v>3049</v>
       </c>
       <c r="I5" t="s">
-        <v>3064</v>
+        <v>3056</v>
       </c>
       <c r="K5" t="s">
-        <v>3054</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="6" spans="2:13">
       <c r="G6" t="s">
-        <v>3062</v>
+        <v>3054</v>
       </c>
       <c r="K6" t="s">
-        <v>3061</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="7" spans="2:13">
       <c r="G7" s="43"/>
       <c r="I7" s="43" t="s">
-        <v>3052</v>
+        <v>3044</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="C8" t="s">
-        <v>3058</v>
+        <v>3050</v>
       </c>
       <c r="G8" s="43"/>
       <c r="I8" s="43" t="s">
-        <v>3053</v>
+        <v>3045</v>
       </c>
       <c r="K8" t="s">
-        <v>3059</v>
+        <v>3051</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -40172,7 +40162,7 @@
         <v>2</v>
       </c>
       <c r="K9" t="s">
-        <v>3060</v>
+        <v>3052</v>
       </c>
       <c r="M9">
         <v>2</v>
@@ -40193,7 +40183,7 @@
     <row r="11" spans="2:13">
       <c r="G11" s="43"/>
       <c r="I11" s="43" t="s">
-        <v>3047</v>
+        <v>3039</v>
       </c>
       <c r="K11" t="s">
         <v>2187</v>
@@ -40216,30 +40206,30 @@
     </row>
     <row r="13" spans="2:13">
       <c r="B13" t="s">
-        <v>3055</v>
+        <v>3047</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="108" customFormat="1"/>
     <row r="22" spans="1:14" ht="15.75" thickBot="1">
       <c r="A22" s="106"/>
-      <c r="B22" s="346" t="s">
+      <c r="B22" s="343" t="s">
         <v>1250</v>
       </c>
-      <c r="C22" s="346"/>
+      <c r="C22" s="343"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106"/>
-      <c r="F22" s="346" t="s">
+      <c r="F22" s="343" t="s">
         <v>1354</v>
       </c>
-      <c r="G22" s="346"/>
-      <c r="H22" s="346"/>
+      <c r="G22" s="343"/>
+      <c r="H22" s="343"/>
       <c r="I22" s="106"/>
       <c r="J22" s="106"/>
-      <c r="K22" s="346" t="s">
+      <c r="K22" s="343" t="s">
         <v>1252</v>
       </c>
-      <c r="L22" s="346"/>
-      <c r="M22" s="346"/>
+      <c r="L22" s="343"/>
+      <c r="M22" s="343"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14">
@@ -40261,7 +40251,7 @@
     <row r="24" spans="1:14">
       <c r="A24" s="106"/>
       <c r="B24" s="84" t="s">
-        <v>3065</v>
+        <v>3057</v>
       </c>
       <c r="C24" s="75"/>
       <c r="D24" s="106"/>
@@ -40319,7 +40309,7 @@
       <c r="J26" s="106"/>
       <c r="K26" s="84"/>
       <c r="L26" s="175" t="s">
-        <v>3066</v>
+        <v>3058</v>
       </c>
       <c r="M26" s="75"/>
       <c r="N26" s="106"/>
@@ -40327,7 +40317,7 @@
     <row r="27" spans="1:14">
       <c r="A27" s="106"/>
       <c r="B27" s="84" t="s">
-        <v>3065</v>
+        <v>3057</v>
       </c>
       <c r="C27" s="75"/>
       <c r="D27" s="106"/>
@@ -40341,7 +40331,7 @@
       <c r="J27" s="106"/>
       <c r="K27" s="84"/>
       <c r="L27" s="175" t="s">
-        <v>3067</v>
+        <v>3059</v>
       </c>
       <c r="M27" s="75"/>
       <c r="N27" s="106"/>
@@ -40349,7 +40339,7 @@
     <row r="28" spans="1:14">
       <c r="A28" s="106"/>
       <c r="B28" s="309" t="s">
-        <v>3067</v>
+        <v>3059</v>
       </c>
       <c r="C28" s="75"/>
       <c r="D28" s="106"/>
@@ -40363,7 +40353,7 @@
       <c r="J28" s="106"/>
       <c r="K28" s="84"/>
       <c r="L28" s="175" t="s">
-        <v>3068</v>
+        <v>3060</v>
       </c>
       <c r="M28" s="75"/>
       <c r="N28" s="106"/>
@@ -40371,7 +40361,7 @@
     <row r="29" spans="1:14">
       <c r="A29" s="106"/>
       <c r="B29" s="309" t="s">
-        <v>3068</v>
+        <v>3060</v>
       </c>
       <c r="C29" s="75"/>
       <c r="D29" s="106"/>
@@ -40407,7 +40397,7 @@
       <c r="J30" s="106"/>
       <c r="K30" s="84"/>
       <c r="L30" s="246" t="s">
-        <v>3066</v>
+        <v>3058</v>
       </c>
       <c r="M30" s="75"/>
       <c r="N30" s="106"/>
@@ -40415,7 +40405,7 @@
     <row r="31" spans="1:14" s="108" customFormat="1">
       <c r="A31" s="106"/>
       <c r="B31" s="84" t="s">
-        <v>3065</v>
+        <v>3057</v>
       </c>
       <c r="C31" s="75"/>
       <c r="D31" s="106"/>
@@ -40445,7 +40435,7 @@
       <c r="J32" s="106"/>
       <c r="K32" s="84"/>
       <c r="L32" s="246" t="s">
-        <v>3066</v>
+        <v>3058</v>
       </c>
       <c r="M32" s="75"/>
       <c r="N32" s="106"/>
@@ -40481,7 +40471,7 @@
       <c r="J34" s="106"/>
       <c r="K34" s="84"/>
       <c r="L34" s="175" t="s">
-        <v>3067</v>
+        <v>3059</v>
       </c>
       <c r="M34" s="75"/>
       <c r="N34" s="106"/>
@@ -40499,7 +40489,7 @@
       <c r="J35" s="106"/>
       <c r="K35" s="84"/>
       <c r="L35" s="175" t="s">
-        <v>3068</v>
+        <v>3060</v>
       </c>
       <c r="M35" s="75"/>
       <c r="N35" s="106"/>
@@ -40555,10 +40545,10 @@
     </row>
     <row r="40" spans="1:16">
       <c r="F40" t="s">
-        <v>3069</v>
+        <v>3061</v>
       </c>
       <c r="H40" t="s">
-        <v>3070</v>
+        <v>3062</v>
       </c>
       <c r="L40" s="244"/>
       <c r="P40" t="s">
@@ -42644,13 +42634,13 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="B1" t="s">
-        <v>3072</v>
+        <v>3064</v>
       </c>
       <c r="C1" t="s">
         <v>2337</v>
       </c>
       <c r="F1" t="s">
-        <v>3072</v>
+        <v>3064</v>
       </c>
       <c r="G1" t="s">
         <v>2337</v>
@@ -42664,7 +42654,7 @@
     </row>
     <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>3071</v>
+        <v>3063</v>
       </c>
       <c r="B2" s="302">
         <v>0</v>
@@ -42790,84 +42780,84 @@
     </row>
     <row r="7" spans="1:31">
       <c r="M7" s="248" t="s">
-        <v>3130</v>
+        <v>3122</v>
       </c>
       <c r="O7">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:31">
-      <c r="B8" s="348" t="s">
-        <v>3073</v>
-      </c>
-      <c r="C8" s="348"/>
-      <c r="F8" s="348" t="s">
-        <v>3074</v>
-      </c>
-      <c r="G8" s="348"/>
-      <c r="I8" s="348" t="s">
-        <v>3074</v>
-      </c>
-      <c r="J8" s="348"/>
+      <c r="B8" s="345" t="s">
+        <v>3065</v>
+      </c>
+      <c r="C8" s="345"/>
+      <c r="F8" s="345" t="s">
+        <v>3066</v>
+      </c>
+      <c r="G8" s="345"/>
+      <c r="I8" s="345" t="s">
+        <v>3066</v>
+      </c>
+      <c r="J8" s="345"/>
       <c r="M8" s="248" t="s">
-        <v>3131</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="9" spans="1:31">
-      <c r="F9" s="348" t="s">
-        <v>3075</v>
-      </c>
-      <c r="G9" s="348"/>
-      <c r="I9" s="348" t="s">
-        <v>3076</v>
-      </c>
-      <c r="J9" s="348"/>
-      <c r="M9" s="349" t="s">
-        <v>3074</v>
-      </c>
-      <c r="N9" s="349"/>
+      <c r="F9" s="345" t="s">
+        <v>3067</v>
+      </c>
+      <c r="G9" s="345"/>
+      <c r="I9" s="345" t="s">
+        <v>3068</v>
+      </c>
+      <c r="J9" s="345"/>
+      <c r="M9" s="346" t="s">
+        <v>3066</v>
+      </c>
+      <c r="N9" s="346"/>
     </row>
     <row r="10" spans="1:31">
       <c r="M10" s="314" t="s">
-        <v>3077</v>
+        <v>3069</v>
       </c>
       <c r="N10" s="314"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="E11" s="347" t="s">
-        <v>3078</v>
-      </c>
-      <c r="F11" s="347"/>
-      <c r="G11" s="347"/>
-      <c r="H11" s="347"/>
-      <c r="I11" s="347"/>
-      <c r="J11" s="347"/>
-      <c r="K11" s="347"/>
-      <c r="L11" s="347"/>
-      <c r="M11" s="347"/>
-      <c r="N11" s="347"/>
-      <c r="O11" s="347"/>
+      <c r="E11" s="344" t="s">
+        <v>3070</v>
+      </c>
+      <c r="F11" s="344"/>
+      <c r="G11" s="344"/>
+      <c r="H11" s="344"/>
+      <c r="I11" s="344"/>
+      <c r="J11" s="344"/>
+      <c r="K11" s="344"/>
+      <c r="L11" s="344"/>
+      <c r="M11" s="344"/>
+      <c r="N11" s="344"/>
+      <c r="O11" s="344"/>
     </row>
     <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>3079</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>3080</v>
+        <v>3072</v>
       </c>
       <c r="F13" t="s">
-        <v>3081</v>
+        <v>3073</v>
       </c>
       <c r="H13" t="s">
-        <v>3082</v>
+        <v>3074</v>
       </c>
       <c r="J13" t="s">
-        <v>3083</v>
+        <v>3075</v>
       </c>
       <c r="L13" t="s">
-        <v>3084</v>
+        <v>3076</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -42999,10 +42989,10 @@
     </row>
     <row r="19" spans="1:32">
       <c r="C19" t="s">
-        <v>3085</v>
+        <v>3077</v>
       </c>
       <c r="F19" t="s">
-        <v>3086</v>
+        <v>3078</v>
       </c>
       <c r="L19" s="27"/>
       <c r="M19" s="43"/>
@@ -43041,7 +43031,7 @@
         <v>412</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>3087</v>
+        <v>3079</v>
       </c>
       <c r="M20" s="174"/>
       <c r="N20" s="27"/>
@@ -43210,7 +43200,7 @@
     </row>
     <row r="26" spans="1:32">
       <c r="F26" s="56" t="s">
-        <v>3088</v>
+        <v>3080</v>
       </c>
       <c r="G26" s="56"/>
       <c r="M26" s="27"/>
@@ -43235,7 +43225,7 @@
     </row>
     <row r="27" spans="1:32">
       <c r="H27" t="s">
-        <v>3102</v>
+        <v>3094</v>
       </c>
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
@@ -43259,10 +43249,10 @@
     </row>
     <row r="28" spans="1:32">
       <c r="A28" t="s">
-        <v>3089</v>
+        <v>3081</v>
       </c>
       <c r="G28" s="43" t="s">
-        <v>3090</v>
+        <v>3082</v>
       </c>
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
@@ -43286,7 +43276,7 @@
     </row>
     <row r="29" spans="1:32">
       <c r="G29" s="43" t="s">
-        <v>3091</v>
+        <v>3083</v>
       </c>
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
@@ -43310,16 +43300,16 @@
     </row>
     <row r="30" spans="1:32" ht="15.75" thickBot="1">
       <c r="E30" t="s">
-        <v>3100</v>
+        <v>3092</v>
       </c>
       <c r="G30" s="159" t="s">
-        <v>3092</v>
+        <v>3084</v>
       </c>
       <c r="I30" t="s">
-        <v>3099</v>
+        <v>3091</v>
       </c>
       <c r="K30" t="s">
-        <v>3098</v>
+        <v>3090</v>
       </c>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
@@ -43344,7 +43334,7 @@
     <row r="31" spans="1:32">
       <c r="E31" s="26"/>
       <c r="G31" s="43" t="s">
-        <v>3093</v>
+        <v>3085</v>
       </c>
       <c r="I31" s="26"/>
       <c r="K31" s="26"/>
@@ -43370,13 +43360,13 @@
     </row>
     <row r="32" spans="1:32">
       <c r="E32" s="312" t="s">
-        <v>3092</v>
+        <v>3084</v>
       </c>
       <c r="G32" s="43" t="s">
-        <v>3094</v>
+        <v>3086</v>
       </c>
       <c r="I32" s="312" t="s">
-        <v>3092</v>
+        <v>3084</v>
       </c>
       <c r="K32" s="312"/>
       <c r="M32" s="27"/>
@@ -43405,7 +43395,7 @@
     <row r="33" spans="1:32">
       <c r="E33" s="312"/>
       <c r="G33" s="43" t="s">
-        <v>3095</v>
+        <v>3087</v>
       </c>
       <c r="I33" s="312"/>
       <c r="K33" s="312"/>
@@ -43435,7 +43425,7 @@
     <row r="34" spans="1:32">
       <c r="E34" s="312"/>
       <c r="G34" s="43" t="s">
-        <v>3096</v>
+        <v>3088</v>
       </c>
       <c r="I34" s="312"/>
       <c r="K34" s="312"/>
@@ -43462,7 +43452,7 @@
     <row r="35" spans="1:32" ht="15.75" thickBot="1">
       <c r="E35" s="212"/>
       <c r="G35" s="43" t="s">
-        <v>3097</v>
+        <v>3089</v>
       </c>
       <c r="I35" s="212"/>
       <c r="K35" s="212"/>
@@ -43509,7 +43499,7 @@
     </row>
     <row r="37" spans="1:32">
       <c r="C37" t="s">
-        <v>3101</v>
+        <v>3093</v>
       </c>
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
@@ -43533,12 +43523,12 @@
     </row>
     <row r="39" spans="1:32">
       <c r="A39" t="s">
-        <v>3103</v>
+        <v>3095</v>
       </c>
     </row>
     <row r="40" spans="1:32">
       <c r="M40" t="s">
-        <v>3109</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="41" spans="1:32">
@@ -43616,7 +43606,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="43" t="s">
-        <v>3106</v>
+        <v>3098</v>
       </c>
     </row>
     <row r="44" spans="1:32">
@@ -43656,7 +43646,7 @@
         <v>99999999</v>
       </c>
       <c r="E45" s="131" t="s">
-        <v>3104</v>
+        <v>3096</v>
       </c>
       <c r="G45">
         <v>99999999</v>
@@ -43676,7 +43666,7 @@
         <v>10000000</v>
       </c>
       <c r="C46" s="131" t="s">
-        <v>3104</v>
+        <v>3096</v>
       </c>
       <c r="D46">
         <v>10000000</v>
@@ -43685,7 +43675,7 @@
         <v>10000000</v>
       </c>
       <c r="H46" s="131" t="s">
-        <v>3104</v>
+        <v>3096</v>
       </c>
       <c r="I46">
         <v>10000000</v>
@@ -43696,15 +43686,15 @@
     </row>
     <row r="47" spans="1:32">
       <c r="J47" s="131" t="s">
-        <v>3104</v>
+        <v>3096</v>
       </c>
     </row>
     <row r="48" spans="1:32">
       <c r="C48" t="s">
-        <v>3086</v>
+        <v>3078</v>
       </c>
       <c r="H48" t="s">
-        <v>3105</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -43868,7 +43858,7 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="56" t="s">
-        <v>3107</v>
+        <v>3099</v>
       </c>
       <c r="B62" s="56"/>
       <c r="N62" s="27"/>
@@ -43990,7 +43980,7 @@
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="56" t="s">
-        <v>3108</v>
+        <v>3100</v>
       </c>
       <c r="B69" s="56"/>
       <c r="N69" s="27"/>
@@ -44065,10 +44055,10 @@
         <v>1908</v>
       </c>
       <c r="C72" s="196" t="s">
-        <v>3028</v>
+        <v>3020</v>
       </c>
       <c r="E72" s="196" t="s">
-        <v>3028</v>
+        <v>3020</v>
       </c>
       <c r="F72" t="s">
         <v>2505</v>
@@ -44111,7 +44101,7 @@
         <v>1908</v>
       </c>
       <c r="D75" t="s">
-        <v>3028</v>
+        <v>3020</v>
       </c>
       <c r="E75" s="196" t="s">
         <v>2505</v>
@@ -44119,7 +44109,7 @@
     </row>
     <row r="77" spans="1:18">
       <c r="B77" t="s">
-        <v>3132</v>
+        <v>3124</v>
       </c>
       <c r="C77" t="s">
         <v>2330</v>
@@ -44133,7 +44123,7 @@
         <v>50</v>
       </c>
       <c r="F78" t="s">
-        <v>3133</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="79" spans="1:18">
@@ -44144,7 +44134,7 @@
         <v>80</v>
       </c>
       <c r="F79" t="s">
-        <v>3134</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="80" spans="1:18">
@@ -44155,7 +44145,7 @@
         <v>20</v>
       </c>
       <c r="L80" t="s">
-        <v>3139</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="81" spans="2:12">
@@ -44169,7 +44159,7 @@
         <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>3135</v>
+        <v>3127</v>
       </c>
       <c r="K81" t="s">
         <v>48</v>
@@ -44182,7 +44172,7 @@
       <c r="B82" s="308"/>
       <c r="C82" s="308"/>
       <c r="F82" t="s">
-        <v>3136</v>
+        <v>3128</v>
       </c>
       <c r="L82" s="308" t="s">
         <v>524</v>
@@ -44198,7 +44188,7 @@
     </row>
     <row r="84" spans="2:12">
       <c r="G84" t="s">
-        <v>3137</v>
+        <v>3129</v>
       </c>
       <c r="L84" s="308" t="s">
         <v>1758</v>
@@ -44209,7 +44199,7 @@
         <v>49</v>
       </c>
       <c r="G85" t="s">
-        <v>3138</v>
+        <v>3130</v>
       </c>
       <c r="L85">
         <v>50</v>
@@ -46165,7 +46155,7 @@
   <sheetData>
     <row r="2" spans="1:21">
       <c r="A2" s="27" t="s">
-        <v>3110</v>
+        <v>3102</v>
       </c>
       <c r="E2" s="121" t="s">
         <v>549</v>
@@ -46181,7 +46171,7 @@
         <v>413</v>
       </c>
       <c r="L2" s="121" t="s">
-        <v>3114</v>
+        <v>3106</v>
       </c>
       <c r="M2" s="122" t="s">
         <v>1152</v>
@@ -46189,7 +46179,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="27" t="s">
-        <v>3111</v>
+        <v>3103</v>
       </c>
       <c r="E3" s="185" t="s">
         <v>550</v>
@@ -46207,7 +46197,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="27" t="s">
-        <v>3112</v>
+        <v>3104</v>
       </c>
       <c r="E4" s="185" t="s">
         <v>709</v>
@@ -46220,7 +46210,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="117" t="s">
-        <v>3113</v>
+        <v>3105</v>
       </c>
       <c r="D5" s="51"/>
       <c r="E5" s="185" t="s">
@@ -46235,10 +46225,10 @@
         <v>1951</v>
       </c>
       <c r="L5" s="121" t="s">
-        <v>3114</v>
+        <v>3106</v>
       </c>
       <c r="M5" s="122" t="s">
-        <v>3115</v>
+        <v>3107</v>
       </c>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
@@ -46260,7 +46250,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="27" t="s">
-        <v>3117</v>
+        <v>3109</v>
       </c>
       <c r="E7" s="185"/>
       <c r="K7" s="117"/>
@@ -46278,10 +46268,10 @@
         <v>2630</v>
       </c>
       <c r="L8" s="121" t="s">
-        <v>3114</v>
+        <v>3106</v>
       </c>
       <c r="M8" s="122" t="s">
-        <v>3116</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -46320,7 +46310,7 @@
         <v>2629</v>
       </c>
       <c r="L11" s="121" t="s">
-        <v>3114</v>
+        <v>3106</v>
       </c>
       <c r="M11" s="122" t="s">
         <v>1152</v>
@@ -46329,7 +46319,7 @@
     <row r="12" spans="1:21">
       <c r="E12" s="185"/>
       <c r="G12" s="27" t="s">
-        <v>3120</v>
+        <v>3112</v>
       </c>
       <c r="K12" s="117"/>
       <c r="L12" s="123" t="s">
@@ -46341,45 +46331,45 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="38" t="s">
-        <v>3119</v>
+        <v>3111</v>
       </c>
       <c r="E13" s="185" t="s">
         <v>2427</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>3118</v>
+        <v>3110</v>
       </c>
       <c r="G13" s="132">
         <v>1</v>
       </c>
       <c r="H13" s="43" t="s">
-        <v>3127</v>
+        <v>3119</v>
       </c>
       <c r="I13" s="43" t="s">
-        <v>3128</v>
+        <v>3120</v>
       </c>
       <c r="M13" s="76"/>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="38" t="s">
-        <v>3122</v>
+        <v>3114</v>
       </c>
       <c r="C14" s="276" t="s">
-        <v>3121</v>
+        <v>3113</v>
       </c>
       <c r="E14" s="185"/>
       <c r="G14" s="132">
         <v>2</v>
       </c>
       <c r="H14" s="43" t="s">
-        <v>3129</v>
+        <v>3121</v>
       </c>
       <c r="I14" s="43"/>
       <c r="M14" s="76"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="38" t="s">
-        <v>3123</v>
+        <v>3115</v>
       </c>
       <c r="E15" s="185"/>
       <c r="G15" s="132"/>
@@ -46389,7 +46379,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="38" t="s">
-        <v>3124</v>
+        <v>3116</v>
       </c>
       <c r="E16" s="123"/>
       <c r="F16" s="256"/>
@@ -46403,7 +46393,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="38" t="s">
-        <v>3125</v>
+        <v>3117</v>
       </c>
       <c r="C17" s="27">
         <f>1</f>
@@ -46412,7 +46402,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="38" t="s">
-        <v>3126</v>
+        <v>3118</v>
       </c>
     </row>
     <row r="39" spans="2:2">
@@ -46606,11 +46596,11 @@
       <c r="L6" s="43" t="s">
         <v>1526</v>
       </c>
-      <c r="M6" s="350" t="s">
+      <c r="M6" s="347" t="s">
         <v>1527</v>
       </c>
-      <c r="N6" s="350"/>
-      <c r="O6" s="350"/>
+      <c r="N6" s="347"/>
+      <c r="O6" s="347"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
@@ -50364,31 +50354,31 @@
     </row>
     <row r="298" spans="3:14">
       <c r="C298" t="s">
-        <v>3193</v>
+        <v>3185</v>
       </c>
       <c r="D298" t="s">
-        <v>3194</v>
+        <v>3186</v>
       </c>
       <c r="E298" t="s">
-        <v>3195</v>
+        <v>3187</v>
       </c>
       <c r="F298" t="s">
-        <v>3196</v>
+        <v>3188</v>
       </c>
       <c r="G298" t="s">
-        <v>3197</v>
+        <v>3189</v>
       </c>
       <c r="H298" t="s">
-        <v>3198</v>
+        <v>3190</v>
       </c>
       <c r="I298" t="s">
-        <v>3199</v>
+        <v>3191</v>
       </c>
       <c r="J298" t="s">
-        <v>3200</v>
+        <v>3192</v>
       </c>
       <c r="L298" t="s">
-        <v>3149</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="299" spans="3:14">
@@ -50487,7 +50477,7 @@
     </row>
     <row r="303" spans="3:14">
       <c r="C303" t="s">
-        <v>3202</v>
+        <v>3194</v>
       </c>
       <c r="D303" s="57"/>
       <c r="E303" s="57"/>
@@ -50499,49 +50489,49 @@
     </row>
     <row r="304" spans="3:14">
       <c r="C304" t="s">
-        <v>3201</v>
+        <v>3193</v>
       </c>
       <c r="G304" t="s">
+        <v>3195</v>
+      </c>
+      <c r="H304" t="s">
+        <v>3196</v>
+      </c>
+      <c r="J304" s="163" t="s">
         <v>3203</v>
-      </c>
-      <c r="H304" t="s">
-        <v>3204</v>
-      </c>
-      <c r="J304" s="163" t="s">
-        <v>3211</v>
       </c>
     </row>
     <row r="305" spans="1:10">
       <c r="G305" t="s">
-        <v>3205</v>
+        <v>3197</v>
       </c>
       <c r="H305" t="s">
-        <v>3206</v>
+        <v>3198</v>
       </c>
       <c r="J305" s="163" t="s">
-        <v>3212</v>
+        <v>3204</v>
       </c>
     </row>
     <row r="306" spans="1:10">
       <c r="G306" t="s">
-        <v>3207</v>
+        <v>3199</v>
       </c>
       <c r="H306" t="s">
-        <v>3208</v>
+        <v>3200</v>
       </c>
       <c r="J306" s="163" t="s">
-        <v>3213</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="307" spans="1:10">
       <c r="G307" t="s">
-        <v>3209</v>
+        <v>3201</v>
       </c>
       <c r="H307" t="s">
-        <v>3210</v>
+        <v>3202</v>
       </c>
       <c r="J307" s="163" t="s">
-        <v>3214</v>
+        <v>3206</v>
       </c>
     </row>
     <row r="311" spans="1:10">
@@ -50551,12 +50541,12 @@
     </row>
     <row r="312" spans="1:10">
       <c r="B312" t="s">
-        <v>3215</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="314" spans="1:10">
       <c r="A314" s="163" t="s">
-        <v>3216</v>
+        <v>3208</v>
       </c>
     </row>
   </sheetData>
@@ -50586,27 +50576,27 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="F1" t="s">
-        <v>3225</v>
+        <v>3217</v>
       </c>
       <c r="J1" t="s">
-        <v>3225</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="30" t="s">
-        <v>3217</v>
+        <v>3209</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>3218</v>
+        <v>3210</v>
       </c>
       <c r="D2" s="32"/>
       <c r="F2" s="30" t="s">
-        <v>3228</v>
+        <v>3220</v>
       </c>
       <c r="G2" s="31"/>
       <c r="H2" s="32"/>
       <c r="J2" s="30" t="s">
-        <v>3223</v>
+        <v>3215</v>
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="32"/>
@@ -50637,14 +50627,14 @@
     <row r="4" spans="1:13">
       <c r="B4" s="33"/>
       <c r="C4" s="27" t="s">
-        <v>3228</v>
+        <v>3220</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>199</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="27" t="s">
-        <v>3223</v>
+        <v>3215</v>
       </c>
       <c r="H4" s="34" t="s">
         <v>183</v>
@@ -50660,14 +50650,14 @@
     <row r="5" spans="1:13">
       <c r="B5" s="33"/>
       <c r="C5" s="38" t="s">
-        <v>3229</v>
+        <v>3221</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>2186</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="27" t="s">
-        <v>3226</v>
+        <v>3218</v>
       </c>
       <c r="H5" s="34" t="s">
         <v>2673</v>
@@ -50683,7 +50673,7 @@
     <row r="6" spans="1:13">
       <c r="B6" s="33"/>
       <c r="C6" s="38" t="s">
-        <v>3223</v>
+        <v>3215</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>183</v>
@@ -50739,24 +50729,24 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1">
       <c r="A11" s="29" t="s">
-        <v>3224</v>
+        <v>3216</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="F11" s="30" t="s">
-        <v>3229</v>
+        <v>3221</v>
       </c>
       <c r="G11" s="31"/>
       <c r="H11" s="32"/>
       <c r="J11" s="30" t="s">
-        <v>3226</v>
+        <v>3218</v>
       </c>
       <c r="K11" s="31"/>
       <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="30" t="s">
-        <v>3219</v>
+        <v>3211</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="32"/>
@@ -50777,7 +50767,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="33" t="s">
-        <v>3220</v>
+        <v>3212</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="34"/>
@@ -50793,7 +50783,7 @@
         <v>180</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>3227</v>
+        <v>3219</v>
       </c>
       <c r="M13" s="40">
         <v>44916</v>
@@ -50801,7 +50791,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="33" t="s">
-        <v>3221</v>
+        <v>3213</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="34"/>
@@ -50810,7 +50800,7 @@
         <v>180</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>3230</v>
+        <v>3222</v>
       </c>
       <c r="J14" s="33"/>
       <c r="K14" s="27" t="s">
@@ -50848,7 +50838,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>3222</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1"/>
@@ -53440,7 +53430,7 @@
         <v>413</v>
       </c>
       <c r="H65" s="27" t="s">
-        <v>3250</v>
+        <v>3242</v>
       </c>
       <c r="I65" s="27"/>
       <c r="J65" s="27" t="s">
@@ -53545,10 +53535,10 @@
     </row>
     <row r="69" spans="1:22">
       <c r="A69" t="s">
-        <v>3241</v>
+        <v>3233</v>
       </c>
       <c r="D69" t="s">
-        <v>3251</v>
+        <v>3243</v>
       </c>
       <c r="F69" s="50" t="s">
         <v>2603</v>
@@ -53574,7 +53564,7 @@
     </row>
     <row r="70" spans="1:22">
       <c r="A70" t="s">
-        <v>3254</v>
+        <v>3246</v>
       </c>
       <c r="F70" s="50" t="s">
         <v>1790</v>
@@ -53600,10 +53590,10 @@
     </row>
     <row r="71" spans="1:22">
       <c r="A71" t="s">
-        <v>3255</v>
+        <v>3247</v>
       </c>
       <c r="F71" s="50" t="s">
-        <v>3253</v>
+        <v>3245</v>
       </c>
       <c r="G71" s="51">
         <v>30</v>
@@ -53626,7 +53616,7 @@
     </row>
     <row r="72" spans="1:22">
       <c r="A72" t="s">
-        <v>3242</v>
+        <v>3234</v>
       </c>
       <c r="F72" s="50" t="s">
         <v>2363</v>
@@ -53652,10 +53642,10 @@
     </row>
     <row r="73" spans="1:22">
       <c r="B73" t="s">
-        <v>3243</v>
+        <v>3235</v>
       </c>
       <c r="F73" s="33" t="s">
-        <v>3252</v>
+        <v>3244</v>
       </c>
       <c r="G73" s="27"/>
       <c r="H73" s="27"/>
@@ -53698,7 +53688,7 @@
     </row>
     <row r="75" spans="1:22">
       <c r="B75" t="s">
-        <v>3244</v>
+        <v>3236</v>
       </c>
       <c r="F75" s="33"/>
       <c r="G75" s="27"/>
@@ -53744,10 +53734,10 @@
     </row>
     <row r="77" spans="1:22">
       <c r="A77" t="s">
-        <v>3245</v>
+        <v>3237</v>
       </c>
       <c r="F77" s="33" t="s">
-        <v>3256</v>
+        <v>3248</v>
       </c>
       <c r="G77" s="27"/>
       <c r="H77" s="27"/>
@@ -53768,10 +53758,10 @@
     </row>
     <row r="78" spans="1:22">
       <c r="B78" t="s">
-        <v>3246</v>
+        <v>3238</v>
       </c>
       <c r="F78" s="33" t="s">
-        <v>3256</v>
+        <v>3248</v>
       </c>
       <c r="G78" s="27"/>
       <c r="H78" s="27"/>
@@ -53795,7 +53785,7 @@
         <v>1780</v>
       </c>
       <c r="F79" s="33" t="s">
-        <v>3256</v>
+        <v>3248</v>
       </c>
       <c r="G79" s="27"/>
       <c r="H79" s="27"/>
@@ -53816,10 +53806,10 @@
     </row>
     <row r="80" spans="1:22">
       <c r="B80" t="s">
-        <v>3247</v>
+        <v>3239</v>
       </c>
       <c r="F80" s="33" t="s">
-        <v>3256</v>
+        <v>3248</v>
       </c>
       <c r="G80" s="27"/>
       <c r="H80" s="27"/>
@@ -53843,7 +53833,7 @@
         <v>144</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>3256</v>
+        <v>3248</v>
       </c>
       <c r="G81" s="27"/>
       <c r="H81" s="27"/>
@@ -53864,10 +53854,10 @@
     </row>
     <row r="82" spans="1:22" ht="15.75" thickBot="1">
       <c r="A82" t="s">
+        <v>3240</v>
+      </c>
+      <c r="F82" s="33" t="s">
         <v>3248</v>
-      </c>
-      <c r="F82" s="33" t="s">
-        <v>3256</v>
       </c>
       <c r="G82" s="27"/>
       <c r="H82" s="36"/>
@@ -53888,7 +53878,7 @@
     </row>
     <row r="83" spans="1:22">
       <c r="B83" t="s">
-        <v>3249</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="84" spans="1:22">

</xml_diff>